<commit_message>
Strings: Solved 8 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="528">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2768,8 +2768,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3651,7 +3651,7 @@
       <c r="B74" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="18"/>
+      <c r="C74" s="17"/>
       <c r="D74" s="8"/>
     </row>
     <row r="75" ht="21" spans="1:4">
@@ -3717,87 +3717,95 @@
       <c r="B80" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C80" s="18"/>
+      <c r="C80" s="17"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" ht="21" spans="1:4">
       <c r="A81" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C81" s="18"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="8"/>
     </row>
     <row r="82" ht="21" spans="1:4">
       <c r="A82" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C82" s="18"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="8"/>
     </row>
     <row r="83" ht="21" spans="1:4">
       <c r="A83" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C83" s="18"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="8"/>
     </row>
     <row r="84" ht="21" spans="1:4">
       <c r="A84" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C84" s="18"/>
+      <c r="C84" s="14"/>
       <c r="D84" s="8"/>
     </row>
     <row r="85" ht="21" spans="1:4">
       <c r="A85" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C85" s="18"/>
+      <c r="C85" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D85" s="8"/>
     </row>
     <row r="86" ht="21" spans="1:4">
       <c r="A86" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C86" s="18"/>
+      <c r="C86" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D86" s="8"/>
     </row>
     <row r="87" ht="21" spans="1:4">
       <c r="A87" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C87" s="18"/>
+      <c r="C87" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D87" s="8"/>
     </row>
     <row r="88" ht="21" spans="1:4">
       <c r="A88" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C88" s="18"/>
+      <c r="C88" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D88" s="8"/>
     </row>
     <row r="89" ht="21" spans="1:4">

</xml_diff>

<commit_message>
Searching & Sorting: Solved 10 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1667,10 +1667,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1759,38 +1759,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1813,52 +1805,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1867,14 +1830,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1889,7 +1845,51 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1940,7 +1940,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1952,175 +2108,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2162,6 +2162,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2171,26 +2186,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2211,6 +2211,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2225,30 +2240,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2259,148 +2250,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2771,8 +2771,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3935,110 +3935,116 @@
       <c r="A101" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C101" s="18"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="8"/>
     </row>
     <row r="102" ht="21" spans="1:4">
       <c r="A102" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C102" s="18"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="8"/>
     </row>
     <row r="103" ht="21" spans="1:4">
       <c r="A103" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C103" s="18"/>
+      <c r="C103" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D103" s="8"/>
     </row>
     <row r="104" ht="21" spans="1:4">
       <c r="A104" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B104" s="13" t="s">
+      <c r="B104" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="C104" s="18"/>
+      <c r="C104" s="14"/>
       <c r="D104" s="8"/>
     </row>
     <row r="105" ht="21" spans="1:4">
       <c r="A105" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B105" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C105" s="18"/>
+      <c r="C105" s="14"/>
       <c r="D105" s="8"/>
     </row>
     <row r="106" ht="21" spans="1:4">
       <c r="A106" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B106" s="13" t="s">
+      <c r="B106" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C106" s="18"/>
+      <c r="C106" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="D106" s="8"/>
     </row>
     <row r="107" ht="21" spans="1:4">
       <c r="A107" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C107" s="18"/>
+      <c r="C107" s="14"/>
       <c r="D107" s="8"/>
     </row>
     <row r="108" ht="21" spans="1:4">
       <c r="A108" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B108" s="13" t="s">
+      <c r="B108" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C108" s="18"/>
+      <c r="C108" s="14"/>
       <c r="D108" s="8"/>
     </row>
     <row r="109" ht="21" spans="1:4">
       <c r="A109" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C109" s="18"/>
+      <c r="C109" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D109" s="8"/>
     </row>
     <row r="110" ht="21" spans="1:4">
       <c r="A110" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B110" s="13" t="s">
+      <c r="B110" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C110" s="18"/>
+      <c r="C110" s="14"/>
       <c r="D110" s="8"/>
     </row>
     <row r="111" ht="21" spans="1:4">
       <c r="A111" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B111" s="13" t="s">
+      <c r="B111" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="C111" s="18"/>
+      <c r="C111" s="14"/>
       <c r="D111" s="8"/>
     </row>
     <row r="112" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[COMPLETE]Searching & Sorting: Solved 9 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="556">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -744,7 +744,7 @@
     <t>Subset Sums</t>
   </si>
   <si>
-    <t>Findthe inversion count</t>
+    <t>Find the inversion count</t>
   </si>
   <si>
     <t>Implement Merge-sort in-place</t>
@@ -2852,8 +2852,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B456" sqref="B456"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -4299,7 +4299,7 @@
       <c r="B122" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C122" s="18"/>
+      <c r="C122" s="17"/>
       <c r="D122" s="8"/>
     </row>
     <row r="123" ht="21" spans="1:4">
@@ -4353,94 +4353,100 @@
       <c r="B127" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C127" s="18"/>
+      <c r="C127" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D127" s="8"/>
     </row>
     <row r="128" ht="21" spans="1:4">
       <c r="A128" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B128" s="13" t="s">
+      <c r="B128" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C128" s="18"/>
+      <c r="C128" s="14"/>
       <c r="D128" s="8"/>
     </row>
     <row r="129" ht="21" spans="1:4">
       <c r="A129" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C129" s="18"/>
+      <c r="C129" s="14"/>
       <c r="D129" s="8"/>
     </row>
     <row r="130" ht="21" spans="1:4">
       <c r="A130" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B130" s="13" t="s">
+      <c r="B130" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C130" s="18"/>
+      <c r="C130" s="14"/>
       <c r="D130" s="8"/>
     </row>
     <row r="131" ht="21" spans="1:4">
       <c r="A131" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B131" s="13" t="s">
+      <c r="B131" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C131" s="18"/>
+      <c r="C131" s="14"/>
       <c r="D131" s="8"/>
     </row>
     <row r="132" ht="21" spans="1:4">
       <c r="A132" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C132" s="18"/>
+      <c r="C132" s="14"/>
       <c r="D132" s="8"/>
     </row>
     <row r="133" ht="21" spans="1:4">
       <c r="A133" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C133" s="18"/>
+      <c r="C133" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D133" s="8"/>
     </row>
     <row r="134" ht="21" spans="1:4">
       <c r="A134" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C134" s="18"/>
+      <c r="C134" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D134" s="8"/>
     </row>
     <row r="135" ht="21" spans="1:4">
       <c r="A135" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B135" s="13" t="s">
+      <c r="B135" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C135" s="18"/>
+      <c r="C135" s="17"/>
       <c r="D135" s="8"/>
     </row>
     <row r="136" ht="21" spans="1:4">
       <c r="A136" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C136" s="18"/>
@@ -7906,7 +7912,7 @@
     <hyperlink ref="B131" r:id="rId112" display="ROTI-Prata SPOJ"/>
     <hyperlink ref="B132" r:id="rId113" display="DoubleHelix SPOJ"/>
     <hyperlink ref="B133" r:id="rId114" display="Subset Sums"/>
-    <hyperlink ref="B134" r:id="rId15" display="Findthe inversion count"/>
+    <hyperlink ref="B134" r:id="rId15" display="Find the inversion count"/>
     <hyperlink ref="B135" r:id="rId115" display="Implement Merge-sort in-place"/>
     <hyperlink ref="B136" r:id="rId116" display="Partitioning and Sorting Arrays with Many Repeated Entries"/>
     <hyperlink ref="B105" r:id="rId117" display="Maximum and minimum of an array using minimum number of comparisons"/>

</xml_diff>

<commit_message>
LinkedList: Completed 8 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1748,9 +1748,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
@@ -1834,7 +1834,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1849,7 +1849,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1862,11 +1870,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1878,9 +1916,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1895,76 +1954,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2021,6 +2021,84 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2033,19 +2111,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2063,139 +2183,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2243,39 +2243,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2287,6 +2254,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2306,16 +2288,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2335,150 +2317,168 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2852,8 +2852,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -4449,7 +4449,7 @@
       <c r="B136" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C136" s="18"/>
+      <c r="C136" s="17"/>
       <c r="D136" s="8"/>
     </row>
     <row r="137" ht="21" spans="3:4">
@@ -4465,17 +4465,17 @@
       <c r="A139" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C139" s="18"/>
+      <c r="C139" s="14"/>
       <c r="D139" s="8"/>
     </row>
     <row r="140" ht="21" spans="1:4">
       <c r="A140" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="B140" s="10" t="s">
         <v>228</v>
       </c>
       <c r="C140" s="18"/>
@@ -4485,40 +4485,40 @@
       <c r="A141" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B141" s="13" t="s">
+      <c r="B141" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="C141" s="18"/>
+      <c r="C141" s="14"/>
       <c r="D141" s="8"/>
     </row>
     <row r="142" ht="21" spans="1:4">
       <c r="A142" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B142" s="13" t="s">
+      <c r="B142" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="C142" s="18"/>
+      <c r="C142" s="14"/>
       <c r="D142" s="8"/>
     </row>
     <row r="143" ht="21" spans="1:4">
       <c r="A143" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B143" s="13" t="s">
+      <c r="B143" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="C143" s="18"/>
+      <c r="C143" s="14"/>
       <c r="D143" s="8"/>
     </row>
     <row r="144" ht="21" spans="1:4">
       <c r="A144" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C144" s="18"/>
+      <c r="C144" s="14"/>
       <c r="D144" s="8"/>
     </row>
     <row r="145" ht="21" spans="1:4">
@@ -4535,17 +4535,17 @@
       <c r="A146" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C146" s="18"/>
+      <c r="C146" s="14"/>
       <c r="D146" s="8"/>
     </row>
     <row r="147" ht="21" spans="1:4">
       <c r="A147" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="10" t="s">
         <v>235</v>
       </c>
       <c r="C147" s="18"/>
@@ -4555,30 +4555,30 @@
       <c r="A148" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B148" s="13" t="s">
+      <c r="B148" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="C148" s="18"/>
+      <c r="C148" s="14"/>
       <c r="D148" s="8"/>
     </row>
     <row r="149" ht="21" spans="1:4">
       <c r="A149" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B149" s="13" t="s">
+      <c r="B149" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C149" s="18"/>
+      <c r="C149" s="14"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" ht="21" spans="1:4">
       <c r="A150" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B150" s="13" t="s">
+      <c r="B150" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="C150" s="18"/>
+      <c r="C150" s="14"/>
       <c r="D150" s="8"/>
     </row>
     <row r="151" ht="21" spans="1:4">

</xml_diff>

<commit_message>
LinkedList: Completed 10 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="556">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2852,8 +2852,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -4478,7 +4478,9 @@
       <c r="B140" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="C140" s="18"/>
+      <c r="C140" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D140" s="8"/>
     </row>
     <row r="141" ht="21" spans="1:4">
@@ -4525,10 +4527,10 @@
       <c r="A145" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C145" s="18"/>
+      <c r="C145" s="14"/>
       <c r="D145" s="8"/>
     </row>
     <row r="146" ht="21" spans="1:4">
@@ -4585,7 +4587,7 @@
       <c r="A151" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B151" s="13" t="s">
+      <c r="B151" s="10" t="s">
         <v>239</v>
       </c>
       <c r="C151" s="18"/>
@@ -4605,80 +4607,86 @@
       <c r="A153" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B153" s="13" t="s">
+      <c r="B153" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C153" s="18"/>
+      <c r="C153" s="14"/>
       <c r="D153" s="8"/>
     </row>
     <row r="154" ht="21" spans="1:4">
       <c r="A154" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B154" s="13" t="s">
+      <c r="B154" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C154" s="18"/>
+      <c r="C154" s="14"/>
       <c r="D154" s="8"/>
     </row>
     <row r="155" ht="21" spans="1:4">
       <c r="A155" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B155" s="13" t="s">
+      <c r="B155" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C155" s="18"/>
+      <c r="C155" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D155" s="8"/>
     </row>
     <row r="156" ht="21" spans="1:4">
       <c r="A156" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B156" s="13" t="s">
+      <c r="B156" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C156" s="18"/>
+      <c r="C156" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D156" s="8"/>
     </row>
     <row r="157" ht="21" spans="1:4">
       <c r="A157" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B157" s="13" t="s">
+      <c r="B157" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C157" s="18"/>
+      <c r="C157" s="14"/>
       <c r="D157" s="8"/>
     </row>
     <row r="158" ht="21" spans="1:4">
       <c r="A158" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B158" s="13" t="s">
+      <c r="B158" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="C158" s="18"/>
+      <c r="C158" s="14"/>
       <c r="D158" s="8"/>
     </row>
     <row r="159" ht="21" spans="1:4">
       <c r="A159" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B159" s="13" t="s">
+      <c r="B159" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C159" s="18"/>
+      <c r="C159" s="14"/>
       <c r="D159" s="8"/>
     </row>
     <row r="160" ht="21" spans="1:4">
       <c r="A160" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B160" s="13" t="s">
+      <c r="B160" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="C160" s="18"/>
+      <c r="C160" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D160" s="8"/>
     </row>
     <row r="161" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[COMPLETE]LinkedList: Solved 10 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="556">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -828,7 +828,7 @@
     <t>Rotate DoublyLinked list by N nodes.</t>
   </si>
   <si>
-    <t>Rotate a Doubly Linked list in group of Given Size.[Very IMP]</t>
+    <t>Reverse a Doubly Linked list in group of Given Size.[Very IMP]</t>
   </si>
   <si>
     <t>Can we reverse a linked list in less than O(n) ?</t>
@@ -2852,8 +2852,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="C160" sqref="C160"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -4693,7 +4693,7 @@
       <c r="A161" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B161" s="13" t="s">
+      <c r="B161" s="10" t="s">
         <v>249</v>
       </c>
       <c r="C161" s="18"/>
@@ -4703,20 +4703,22 @@
       <c r="A162" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B162" s="13" t="s">
+      <c r="B162" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C162" s="18"/>
+      <c r="C162" s="14"/>
       <c r="D162" s="8"/>
     </row>
     <row r="163" ht="21" spans="1:4">
       <c r="A163" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B163" s="13" t="s">
+      <c r="B163" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C163" s="18"/>
+      <c r="C163" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D163" s="8"/>
     </row>
     <row r="164" ht="21" spans="1:4">
@@ -4743,90 +4745,102 @@
       <c r="A166" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B166" s="13" t="s">
+      <c r="B166" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C166" s="18"/>
+      <c r="C166" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D166" s="8"/>
     </row>
     <row r="167" ht="21" spans="1:4">
       <c r="A167" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B167" s="13" t="s">
+      <c r="B167" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="C167" s="18"/>
+      <c r="C167" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D167" s="8"/>
     </row>
     <row r="168" ht="21" spans="1:4">
       <c r="A168" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B168" s="13" t="s">
+      <c r="B168" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C168" s="18"/>
+      <c r="C168" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D168" s="8"/>
     </row>
     <row r="169" ht="21" spans="1:4">
       <c r="A169" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B169" s="13" t="s">
+      <c r="B169" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C169" s="18"/>
+      <c r="C169" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="D169" s="8"/>
     </row>
     <row r="170" ht="21" spans="1:4">
       <c r="A170" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B170" s="13" t="s">
+      <c r="B170" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C170" s="18"/>
+      <c r="C170" s="14"/>
       <c r="D170" s="8"/>
     </row>
     <row r="171" ht="21" spans="1:4">
       <c r="A171" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B171" s="13" t="s">
+      <c r="B171" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="C171" s="18"/>
+      <c r="C171" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D171" s="8"/>
     </row>
     <row r="172" ht="21" spans="1:4">
       <c r="A172" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B172" s="13" t="s">
+      <c r="B172" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C172" s="18"/>
+      <c r="C172" s="14"/>
       <c r="D172" s="8"/>
     </row>
     <row r="173" ht="21" spans="1:4">
       <c r="A173" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B173" s="13" t="s">
+      <c r="B173" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C173" s="18"/>
+      <c r="C173" s="14"/>
       <c r="D173" s="8"/>
     </row>
     <row r="174" ht="21" spans="1:4">
       <c r="A174" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B174" s="13" t="s">
+      <c r="B174" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C174" s="18"/>
+      <c r="C174" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D174" s="8"/>
     </row>
     <row r="175" ht="21" spans="3:4">
@@ -7949,7 +7963,7 @@
     <hyperlink ref="B160" r:id="rId140" display="Count triplets in a sorted DLL whose sum is equal to given value “X”."/>
     <hyperlink ref="B161" r:id="rId141" display="Sort a “k”sorted Doubly Linked list.[Very IMP]"/>
     <hyperlink ref="B162" r:id="rId142" display="Rotate DoublyLinked list by N nodes."/>
-    <hyperlink ref="B163" r:id="rId143" display="Rotate a Doubly Linked list in group of Given Size.[Very IMP]"/>
+    <hyperlink ref="B163" r:id="rId143" display="Reverse a Doubly Linked list in group of Given Size.[Very IMP]"/>
     <hyperlink ref="B166" r:id="rId144" display="Flatten a Linked List"/>
     <hyperlink ref="B167" r:id="rId145" display="Sort a LL of 0's, 1's and 2's"/>
     <hyperlink ref="B168" r:id="rId146" display="Clone a linked list with next and random pointer"/>

</xml_diff>

<commit_message>
BinaryTrees: Solved 14 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2984,8 +2984,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3087,7 +3087,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5182,37 +5182,39 @@
       <c r="A187" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B187" s="13" t="s">
+      <c r="B187" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="C187" s="18"/>
+      <c r="C187" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D187" s="8"/>
     </row>
     <row r="188" ht="21" spans="1:4">
       <c r="A188" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B188" s="13" t="s">
+      <c r="B188" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="C188" s="18"/>
+      <c r="C188" s="14"/>
       <c r="D188" s="8"/>
     </row>
     <row r="189" ht="21" spans="1:4">
       <c r="A189" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B189" s="13" t="s">
+      <c r="B189" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C189" s="18"/>
+      <c r="C189" s="14"/>
       <c r="D189" s="8"/>
     </row>
     <row r="190" ht="21" spans="1:4">
       <c r="A190" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B190" s="13" t="s">
+      <c r="B190" s="10" t="s">
         <v>321</v>
       </c>
       <c r="C190" s="18"/>
@@ -5222,7 +5224,7 @@
       <c r="A191" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B191" s="13" t="s">
+      <c r="B191" s="10" t="s">
         <v>322</v>
       </c>
       <c r="C191" s="18"/>
@@ -5232,7 +5234,7 @@
       <c r="A192" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B192" s="13" t="s">
+      <c r="B192" s="10" t="s">
         <v>323</v>
       </c>
       <c r="C192" s="18"/>
@@ -5242,7 +5244,7 @@
       <c r="A193" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B193" s="13" t="s">
+      <c r="B193" s="10" t="s">
         <v>324</v>
       </c>
       <c r="C193" s="18"/>
@@ -5252,7 +5254,7 @@
       <c r="A194" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B194" s="13" t="s">
+      <c r="B194" s="10" t="s">
         <v>325</v>
       </c>
       <c r="C194" s="18"/>
@@ -5262,7 +5264,7 @@
       <c r="A195" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B195" s="13" t="s">
+      <c r="B195" s="10" t="s">
         <v>326</v>
       </c>
       <c r="C195" s="18"/>
@@ -5272,7 +5274,7 @@
       <c r="A196" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B196" s="13" t="s">
+      <c r="B196" s="10" t="s">
         <v>327</v>
       </c>
       <c r="C196" s="18"/>
@@ -5282,7 +5284,7 @@
       <c r="A197" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B197" s="13" t="s">
+      <c r="B197" s="10" t="s">
         <v>328</v>
       </c>
       <c r="C197" s="18"/>
@@ -5292,7 +5294,7 @@
       <c r="A198" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B198" s="13" t="s">
+      <c r="B198" s="10" t="s">
         <v>329</v>
       </c>
       <c r="C198" s="18"/>
@@ -5302,7 +5304,7 @@
       <c r="A199" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B199" s="13" t="s">
+      <c r="B199" s="10" t="s">
         <v>330</v>
       </c>
       <c r="C199" s="18"/>
@@ -5312,7 +5314,7 @@
       <c r="A200" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B200" s="13" t="s">
+      <c r="B200" s="10" t="s">
         <v>331</v>
       </c>
       <c r="C200" s="18"/>
@@ -5322,7 +5324,7 @@
       <c r="A201" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B201" s="13" t="s">
+      <c r="B201" s="10" t="s">
         <v>332</v>
       </c>
       <c r="C201" s="18"/>
@@ -5332,7 +5334,7 @@
       <c r="A202" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B202" s="13" t="s">
+      <c r="B202" s="10" t="s">
         <v>333</v>
       </c>
       <c r="C202" s="18"/>
@@ -5342,7 +5344,7 @@
       <c r="A203" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B203" s="13" t="s">
+      <c r="B203" s="10" t="s">
         <v>334</v>
       </c>
       <c r="C203" s="18"/>

</xml_diff>

<commit_message>
[COMPLETE]BinaryTrees: Solved 10 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2984,8 +2984,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="C211" sqref="C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5217,7 +5217,7 @@
       <c r="B190" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="C190" s="18"/>
+      <c r="C190" s="14"/>
       <c r="D190" s="8"/>
     </row>
     <row r="191" ht="21" spans="1:4">
@@ -5227,7 +5227,9 @@
       <c r="B191" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="C191" s="18"/>
+      <c r="C191" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D191" s="8"/>
     </row>
     <row r="192" ht="21" spans="1:4">
@@ -5237,7 +5239,9 @@
       <c r="B192" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="C192" s="18"/>
+      <c r="C192" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D192" s="8"/>
     </row>
     <row r="193" ht="21" spans="1:4">
@@ -5247,7 +5251,9 @@
       <c r="B193" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="C193" s="18"/>
+      <c r="C193" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D193" s="8"/>
     </row>
     <row r="194" ht="21" spans="1:4">
@@ -5257,7 +5263,9 @@
       <c r="B194" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="C194" s="18"/>
+      <c r="C194" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D194" s="8"/>
     </row>
     <row r="195" ht="21" spans="1:4">
@@ -5267,7 +5275,7 @@
       <c r="B195" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="C195" s="18"/>
+      <c r="C195" s="14"/>
       <c r="D195" s="8"/>
     </row>
     <row r="196" ht="21" spans="1:4">
@@ -5277,7 +5285,7 @@
       <c r="B196" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="C196" s="18"/>
+      <c r="C196" s="14"/>
       <c r="D196" s="8"/>
     </row>
     <row r="197" ht="21" spans="1:4">
@@ -5287,7 +5295,7 @@
       <c r="B197" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="C197" s="18"/>
+      <c r="C197" s="14"/>
       <c r="D197" s="8"/>
     </row>
     <row r="198" ht="21" spans="1:4">
@@ -5297,7 +5305,7 @@
       <c r="B198" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="C198" s="18"/>
+      <c r="C198" s="14"/>
       <c r="D198" s="8"/>
     </row>
     <row r="199" ht="21" spans="1:4">
@@ -5307,7 +5315,7 @@
       <c r="B199" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="C199" s="18"/>
+      <c r="C199" s="14"/>
       <c r="D199" s="8"/>
     </row>
     <row r="200" ht="21" spans="1:4">
@@ -5317,7 +5325,7 @@
       <c r="B200" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="C200" s="18"/>
+      <c r="C200" s="14"/>
       <c r="D200" s="8"/>
     </row>
     <row r="201" ht="21" spans="1:4">
@@ -5327,7 +5335,7 @@
       <c r="B201" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="C201" s="18"/>
+      <c r="C201" s="14"/>
       <c r="D201" s="8"/>
     </row>
     <row r="202" ht="21" spans="1:4">
@@ -5337,7 +5345,7 @@
       <c r="B202" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="C202" s="18"/>
+      <c r="C202" s="14"/>
       <c r="D202" s="8"/>
     </row>
     <row r="203" ht="21" spans="1:4">
@@ -5347,87 +5355,95 @@
       <c r="B203" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C203" s="18"/>
+      <c r="C203" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D203" s="8"/>
     </row>
     <row r="204" ht="21" spans="1:4">
       <c r="A204" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B204" s="13" t="s">
+      <c r="B204" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="C204" s="18"/>
+      <c r="C204" s="14"/>
       <c r="D204" s="8"/>
     </row>
     <row r="205" ht="21" spans="1:4">
       <c r="A205" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B205" s="13" t="s">
+      <c r="B205" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="C205" s="18"/>
+      <c r="C205" s="14"/>
       <c r="D205" s="8"/>
     </row>
     <row r="206" ht="21" spans="1:4">
       <c r="A206" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B206" s="13" t="s">
+      <c r="B206" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="C206" s="18"/>
+      <c r="C206" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D206" s="8"/>
     </row>
     <row r="207" ht="21" spans="1:4">
       <c r="A207" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B207" s="13" t="s">
+      <c r="B207" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="C207" s="18"/>
+      <c r="C207" s="14"/>
       <c r="D207" s="8"/>
     </row>
     <row r="208" ht="21" spans="1:4">
       <c r="A208" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B208" s="13" t="s">
+      <c r="B208" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="C208" s="18"/>
+      <c r="C208" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D208" s="8"/>
     </row>
     <row r="209" ht="21" spans="1:4">
       <c r="A209" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B209" s="13" t="s">
+      <c r="B209" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C209" s="18"/>
+      <c r="C209" s="14"/>
       <c r="D209" s="8"/>
     </row>
     <row r="210" ht="21" spans="1:4">
       <c r="A210" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B210" s="13" t="s">
+      <c r="B210" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="C210" s="18"/>
+      <c r="C210" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D210" s="8"/>
     </row>
     <row r="211" ht="21" spans="1:4">
       <c r="A211" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B211" s="13" t="s">
+      <c r="B211" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="C211" s="18"/>
+      <c r="C211" s="14"/>
       <c r="D211" s="8"/>
     </row>
     <row r="212" ht="21" spans="1:4">

</xml_diff>

<commit_message>
BinarySearchTree: Solved 13 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1137,7 +1137,7 @@
     <t>Convert a normal BST into a Balanced BST</t>
   </si>
   <si>
-    <t>Merge two BST [ V.V.V&gt;IMP ]</t>
+    <t>Merge two BST [ V.V.V IMP ]</t>
   </si>
   <si>
     <t>Find Kth largest element in a BST</t>
@@ -1973,40 +1973,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2018,7 +1987,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2041,7 +2032,53 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2049,14 +2086,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2070,41 +2100,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2153,25 +2153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2183,7 +2165,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2201,25 +2189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2231,13 +2201,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2249,7 +2225,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2261,25 +2249,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2291,7 +2267,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2303,13 +2285,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2327,13 +2303,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2375,15 +2375,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2414,21 +2405,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2444,16 +2420,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2472,124 +2439,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2598,19 +2598,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2618,7 +2618,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2659,6 +2659,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2984,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="C211" sqref="C211"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5462,60 +5465,60 @@
       <c r="A214" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B214" s="13" t="s">
+      <c r="B214" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="C214" s="18"/>
+      <c r="C214" s="14"/>
       <c r="D214" s="8"/>
     </row>
     <row r="215" ht="21" spans="1:4">
       <c r="A215" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B215" s="13" t="s">
+      <c r="B215" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="C215" s="18"/>
+      <c r="C215" s="14"/>
       <c r="D215" s="8"/>
     </row>
     <row r="216" ht="21" spans="1:4">
       <c r="A216" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B216" s="13" t="s">
+      <c r="B216" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="C216" s="18"/>
+      <c r="C216" s="14"/>
       <c r="D216" s="8"/>
     </row>
     <row r="217" ht="21" spans="1:4">
       <c r="A217" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B217" s="13" t="s">
+      <c r="B217" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C217" s="18"/>
+      <c r="C217" s="14"/>
       <c r="D217" s="8"/>
     </row>
     <row r="218" ht="21" spans="1:4">
       <c r="A218" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B218" s="13" t="s">
+      <c r="B218" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="C218" s="18"/>
+      <c r="C218" s="14"/>
       <c r="D218" s="8"/>
     </row>
     <row r="219" ht="21" spans="1:4">
       <c r="A219" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B219" s="13" t="s">
+      <c r="B219" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C219" s="18"/>
+      <c r="C219" s="14"/>
       <c r="D219" s="8"/>
     </row>
     <row r="220" ht="21" spans="1:4">
@@ -5525,17 +5528,17 @@
       <c r="B220" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="C220" s="18"/>
+      <c r="C220" s="14"/>
       <c r="D220" s="8"/>
     </row>
     <row r="221" ht="21" spans="1:4">
       <c r="A221" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B221" s="13" t="s">
+      <c r="B221" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="C221" s="18"/>
+      <c r="C221" s="14"/>
       <c r="D221" s="8"/>
     </row>
     <row r="222" ht="21" spans="1:4">
@@ -5572,20 +5575,20 @@
       <c r="A225" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B225" s="13" t="s">
+      <c r="B225" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="C225" s="18"/>
+      <c r="C225" s="14"/>
       <c r="D225" s="8"/>
     </row>
     <row r="226" ht="21" spans="1:4">
       <c r="A226" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B226" s="13" t="s">
+      <c r="B226" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="C226" s="18"/>
+      <c r="C226" s="14"/>
       <c r="D226" s="8"/>
     </row>
     <row r="227" ht="21" spans="1:4">
@@ -5672,10 +5675,12 @@
       <c r="A235" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B235" s="13" t="s">
+      <c r="B235" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C235" s="18"/>
+      <c r="C235" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D235" s="8"/>
     </row>
     <row r="236" ht="21" spans="2:4">
@@ -6382,7 +6387,7 @@
       <c r="A309" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B309" s="19" t="s">
+      <c r="B309" s="20" t="s">
         <v>435</v>
       </c>
       <c r="C309" s="18"/>
@@ -6722,7 +6727,7 @@
       <c r="A344" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B344" s="19" t="s">
+      <c r="B344" s="20" t="s">
         <v>469</v>
       </c>
       <c r="C344" s="18"/>
@@ -8262,7 +8267,7 @@
     <hyperlink ref="B221" r:id="rId195" display="Construct BST from preorder traversal"/>
     <hyperlink ref="B222" r:id="rId196" display="Convert Binary tree into BST"/>
     <hyperlink ref="B223" r:id="rId197" display="Convert a normal BST into a Balanced BST"/>
-    <hyperlink ref="B224" r:id="rId198" display="Merge two BST [ V.V.V&gt;IMP ]"/>
+    <hyperlink ref="B224" r:id="rId198" display="Merge two BST [ V.V.V IMP ]"/>
     <hyperlink ref="B225" r:id="rId199" display="Find Kth largest element in a BST"/>
     <hyperlink ref="B226" r:id="rId200" display="Find Kth smallest element in a BST"/>
     <hyperlink ref="B227" r:id="rId201" display="Count pairs from 2 BST whose sum is equal to given value &quot;X&quot;"/>

</xml_diff>

<commit_message>
[COMPLETE]BinarySearchTrees: Solved 12 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5545,30 +5545,32 @@
       <c r="A222" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B222" s="13" t="s">
+      <c r="B222" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="C222" s="18"/>
+      <c r="C222" s="14"/>
       <c r="D222" s="8"/>
     </row>
     <row r="223" ht="21" spans="1:4">
       <c r="A223" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B223" s="13" t="s">
+      <c r="B223" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="C223" s="18"/>
+      <c r="C223" s="14"/>
       <c r="D223" s="8"/>
     </row>
     <row r="224" ht="21" spans="1:4">
       <c r="A224" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B224" s="13" t="s">
+      <c r="B224" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="C224" s="18"/>
+      <c r="C224" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D224" s="8"/>
     </row>
     <row r="225" ht="21" spans="1:4">
@@ -5595,47 +5597,51 @@
       <c r="A227" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B227" s="13" t="s">
+      <c r="B227" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="C227" s="18"/>
+      <c r="C227" s="14"/>
       <c r="D227" s="8"/>
     </row>
     <row r="228" ht="21" spans="1:4">
       <c r="A228" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B228" s="13" t="s">
+      <c r="B228" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C228" s="18"/>
+      <c r="C228" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D228" s="8"/>
     </row>
     <row r="229" ht="21" spans="1:4">
       <c r="A229" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B229" s="13" t="s">
+      <c r="B229" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="C229" s="18"/>
+      <c r="C229" s="14"/>
       <c r="D229" s="8"/>
     </row>
     <row r="230" ht="21" spans="1:4">
       <c r="A230" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B230" s="13" t="s">
+      <c r="B230" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="C230" s="18"/>
+      <c r="C230" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D230" s="8"/>
     </row>
     <row r="231" ht="21" spans="1:4">
       <c r="A231" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B231" s="13" t="s">
+      <c r="B231" s="10" t="s">
         <v>361</v>
       </c>
       <c r="C231" s="18"/>
@@ -5645,7 +5651,7 @@
       <c r="A232" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B232" s="13" t="s">
+      <c r="B232" s="10" t="s">
         <v>362</v>
       </c>
       <c r="C232" s="18"/>
@@ -5655,20 +5661,22 @@
       <c r="A233" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B233" s="13" t="s">
+      <c r="B233" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="C233" s="18"/>
+      <c r="C233" s="14"/>
       <c r="D233" s="8"/>
     </row>
     <row r="234" ht="21" spans="1:4">
       <c r="A234" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B234" s="13" t="s">
+      <c r="B234" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="C234" s="18"/>
+      <c r="C234" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D234" s="8"/>
     </row>
     <row r="235" ht="21" spans="1:4">

</xml_diff>

<commit_message>
Greedy: Solved 11 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5654,7 +5654,7 @@
       <c r="B232" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="C232" s="18"/>
+      <c r="C232" s="14"/>
       <c r="D232" s="8"/>
     </row>
     <row r="233" ht="21" spans="1:4">
@@ -5705,100 +5705,116 @@
       <c r="A238" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B238" s="13" t="s">
+      <c r="B238" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C238" s="18"/>
+      <c r="C238" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D238" s="8"/>
     </row>
     <row r="239" ht="21" spans="1:4">
       <c r="A239" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B239" s="13" t="s">
+      <c r="B239" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="C239" s="18"/>
+      <c r="C239" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D239" s="8"/>
     </row>
     <row r="240" ht="21" spans="1:4">
       <c r="A240" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B240" s="13" t="s">
+      <c r="B240" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="C240" s="18"/>
+      <c r="C240" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D240" s="8"/>
     </row>
     <row r="241" ht="21" spans="1:4">
       <c r="A241" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B241" s="13" t="s">
+      <c r="B241" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="C241" s="18"/>
+      <c r="C241" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D241" s="8"/>
     </row>
     <row r="242" ht="21" spans="1:4">
       <c r="A242" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B242" s="13" t="s">
+      <c r="B242" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C242" s="18"/>
+      <c r="C242" s="14"/>
       <c r="D242" s="8"/>
     </row>
     <row r="243" ht="21" spans="1:4">
       <c r="A243" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B243" s="13" t="s">
+      <c r="B243" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="C243" s="18"/>
+      <c r="C243" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D243" s="8"/>
     </row>
     <row r="244" ht="21" spans="1:4">
       <c r="A244" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B244" s="13" t="s">
+      <c r="B244" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="C244" s="18"/>
+      <c r="C244" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D244" s="8"/>
     </row>
     <row r="245" ht="21" spans="1:4">
       <c r="A245" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B245" s="13" t="s">
+      <c r="B245" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="C245" s="18"/>
+      <c r="C245" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D245" s="8"/>
     </row>
     <row r="246" ht="21" spans="1:4">
       <c r="A246" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B246" s="13" t="s">
+      <c r="B246" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C246" s="18"/>
+      <c r="C246" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D246" s="8"/>
     </row>
     <row r="247" ht="21" spans="1:4">
       <c r="A247" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B247" s="13" t="s">
+      <c r="B247" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="C247" s="18"/>
+      <c r="C247" s="14"/>
       <c r="D247" s="8"/>
     </row>
     <row r="248" ht="21" spans="1:4">

</xml_diff>

<commit_message>
Greedy: Solved 10 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1880,9 +1880,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
@@ -1972,10 +1972,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1986,30 +1995,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2024,7 +2012,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2039,46 +2086,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2097,14 +2105,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2153,25 +2153,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2189,7 +2201,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2201,13 +2249,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2219,49 +2279,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2279,13 +2309,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2297,37 +2327,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2375,6 +2375,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2407,10 +2431,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2418,24 +2440,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2463,154 +2472,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5821,7 +5821,7 @@
       <c r="A248" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B248" s="13" t="s">
+      <c r="B248" s="10" t="s">
         <v>377</v>
       </c>
       <c r="C248" s="18"/>
@@ -5831,7 +5831,7 @@
       <c r="A249" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B249" s="13" t="s">
+      <c r="B249" s="10" t="s">
         <v>378</v>
       </c>
       <c r="C249" s="18"/>
@@ -5841,87 +5841,91 @@
       <c r="A250" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B250" s="13" t="s">
+      <c r="B250" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="C250" s="18"/>
+      <c r="C250" s="14"/>
       <c r="D250" s="8"/>
     </row>
     <row r="251" ht="21" spans="1:4">
       <c r="A251" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B251" s="13" t="s">
+      <c r="B251" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="C251" s="18"/>
+      <c r="C251" s="14"/>
       <c r="D251" s="8"/>
     </row>
     <row r="252" ht="21" spans="1:4">
       <c r="A252" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B252" s="13" t="s">
+      <c r="B252" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="C252" s="18"/>
+      <c r="C252" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D252" s="8"/>
     </row>
     <row r="253" ht="21" spans="1:4">
       <c r="A253" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B253" s="13" t="s">
+      <c r="B253" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="C253" s="18"/>
+      <c r="C253" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D253" s="8"/>
     </row>
     <row r="254" ht="21" spans="1:4">
       <c r="A254" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B254" s="13" t="s">
+      <c r="B254" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="C254" s="18"/>
+      <c r="C254" s="14"/>
       <c r="D254" s="8"/>
     </row>
     <row r="255" ht="21" spans="1:4">
       <c r="A255" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B255" s="13" t="s">
+      <c r="B255" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C255" s="18"/>
+      <c r="C255" s="14"/>
       <c r="D255" s="8"/>
     </row>
     <row r="256" ht="21" spans="1:4">
       <c r="A256" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B256" s="13" t="s">
+      <c r="B256" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="C256" s="18"/>
+      <c r="C256" s="14"/>
       <c r="D256" s="8"/>
     </row>
     <row r="257" ht="21" spans="1:4">
       <c r="A257" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B257" s="13" t="s">
+      <c r="B257" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="C257" s="18"/>
+      <c r="C257" s="14"/>
       <c r="D257" s="8"/>
     </row>
     <row r="258" ht="21" spans="1:4">
       <c r="A258" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B258" s="13" t="s">
+      <c r="B258" s="10" t="s">
         <v>387</v>
       </c>
       <c r="C258" s="18"/>
@@ -5941,10 +5945,10 @@
       <c r="A260" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B260" s="13" t="s">
+      <c r="B260" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="C260" s="18"/>
+      <c r="C260" s="14"/>
       <c r="D260" s="8"/>
     </row>
     <row r="261" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[COMPLETE]Greedy: Solved 10 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1880,10 +1880,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1972,9 +1972,115 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1989,75 +2095,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2065,44 +2103,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2153,7 +2153,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2165,7 +2285,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2177,25 +2303,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2207,133 +2327,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2375,15 +2375,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2395,6 +2386,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2414,30 +2414,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2445,15 +2421,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2472,145 +2439,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -5928,7 +5928,9 @@
       <c r="B258" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C258" s="18"/>
+      <c r="C258" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D258" s="8"/>
     </row>
     <row r="259" ht="21" spans="1:4">
@@ -5955,47 +5957,51 @@
       <c r="A261" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B261" s="13" t="s">
+      <c r="B261" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="C261" s="18"/>
+      <c r="C261" s="14"/>
       <c r="D261" s="8"/>
     </row>
     <row r="262" ht="21" spans="1:4">
       <c r="A262" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B262" s="13" t="s">
+      <c r="B262" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="C262" s="18"/>
+      <c r="C262" s="14"/>
       <c r="D262" s="8"/>
     </row>
     <row r="263" ht="21" spans="1:4">
       <c r="A263" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B263" s="13" t="s">
+      <c r="B263" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="C263" s="18"/>
+      <c r="C263" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D263" s="8"/>
     </row>
     <row r="264" ht="21" spans="1:4">
       <c r="A264" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B264" s="13" t="s">
+      <c r="B264" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="C264" s="18"/>
+      <c r="C264" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D264" s="8"/>
     </row>
     <row r="265" ht="21" spans="1:4">
       <c r="A265" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B265" s="13" t="s">
+      <c r="B265" s="10" t="s">
         <v>394</v>
       </c>
       <c r="C265" s="18"/>
@@ -6005,17 +6011,19 @@
       <c r="A266" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B266" s="13" t="s">
+      <c r="B266" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="C266" s="18"/>
+      <c r="C266" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D266" s="8"/>
     </row>
     <row r="267" ht="21" spans="1:4">
       <c r="A267" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B267" s="13" t="s">
+      <c r="B267" s="10" t="s">
         <v>396</v>
       </c>
       <c r="C267" s="18"/>
@@ -6025,7 +6033,7 @@
       <c r="A268" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B268" s="13" t="s">
+      <c r="B268" s="10" t="s">
         <v>397</v>
       </c>
       <c r="C268" s="18"/>
@@ -6035,40 +6043,42 @@
       <c r="A269" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B269" s="13" t="s">
+      <c r="B269" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="C269" s="18"/>
+      <c r="C269" s="14"/>
       <c r="D269" s="8"/>
     </row>
     <row r="270" ht="21" spans="1:4">
       <c r="A270" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B270" s="13" t="s">
+      <c r="B270" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="C270" s="18"/>
+      <c r="C270" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D270" s="8"/>
     </row>
     <row r="271" ht="21" spans="1:4">
       <c r="A271" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B271" s="13" t="s">
+      <c r="B271" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C271" s="18"/>
+      <c r="C271" s="14"/>
       <c r="D271" s="8"/>
     </row>
     <row r="272" ht="21" spans="1:4">
       <c r="A272" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B272" s="13" t="s">
+      <c r="B272" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="C272" s="18"/>
+      <c r="C272" s="14"/>
       <c r="D272" s="8"/>
     </row>
     <row r="273" ht="21" spans="2:4">

</xml_diff>

<commit_message>
[COMPLETE]Backtracking: Solved 17 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1880,10 +1880,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1972,47 +1972,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2026,31 +1995,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2072,10 +2026,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2086,8 +2064,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2102,7 +2094,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2153,19 +2153,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2177,7 +2171,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2189,13 +2183,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2207,25 +2231,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2237,13 +2249,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2261,7 +2273,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2273,7 +2309,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2285,55 +2333,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2390,15 +2390,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2416,11 +2407,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2442,9 +2446,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2458,159 +2464,153 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="C293" sqref="C293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6095,57 +6095,65 @@
       <c r="A275" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B275" s="13" t="s">
+      <c r="B275" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="C275" s="18"/>
+      <c r="C275" s="14"/>
       <c r="D275" s="8"/>
     </row>
     <row r="276" ht="21" spans="1:4">
       <c r="A276" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B276" s="13" t="s">
+      <c r="B276" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C276" s="18"/>
+      <c r="C276" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D276" s="8"/>
     </row>
     <row r="277" ht="21" spans="1:4">
       <c r="A277" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B277" s="13" t="s">
+      <c r="B277" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="C277" s="18"/>
+      <c r="C277" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D277" s="8"/>
     </row>
     <row r="278" ht="21" spans="1:4">
       <c r="A278" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B278" s="13" t="s">
+      <c r="B278" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="C278" s="18"/>
+      <c r="C278" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D278" s="8"/>
     </row>
     <row r="279" ht="21" spans="1:4">
       <c r="A279" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B279" s="13" t="s">
+      <c r="B279" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C279" s="18"/>
+      <c r="C279" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D279" s="8"/>
     </row>
     <row r="280" ht="21" spans="1:4">
       <c r="A280" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B280" s="13" t="s">
+      <c r="B280" s="10" t="s">
         <v>407</v>
       </c>
       <c r="C280" s="18"/>
@@ -6155,27 +6163,29 @@
       <c r="A281" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B281" s="13" t="s">
+      <c r="B281" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="C281" s="18"/>
+      <c r="C281" s="14"/>
       <c r="D281" s="8"/>
     </row>
     <row r="282" ht="21" spans="1:4">
       <c r="A282" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B282" s="13" t="s">
+      <c r="B282" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="C282" s="18"/>
+      <c r="C282" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D282" s="8"/>
     </row>
     <row r="283" ht="21" spans="1:4">
       <c r="A283" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B283" s="13" t="s">
+      <c r="B283" s="10" t="s">
         <v>410</v>
       </c>
       <c r="C283" s="18"/>
@@ -6185,7 +6195,7 @@
       <c r="A284" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B284" s="13" t="s">
+      <c r="B284" s="10" t="s">
         <v>411</v>
       </c>
       <c r="C284" s="18"/>
@@ -6195,7 +6205,7 @@
       <c r="A285" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B285" s="13" t="s">
+      <c r="B285" s="10" t="s">
         <v>412</v>
       </c>
       <c r="C285" s="18"/>
@@ -6205,37 +6215,39 @@
       <c r="A286" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B286" s="13" t="s">
+      <c r="B286" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="C286" s="18"/>
+      <c r="C286" s="14"/>
       <c r="D286" s="8"/>
     </row>
     <row r="287" ht="21" spans="1:4">
       <c r="A287" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B287" s="13" t="s">
+      <c r="B287" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="C287" s="18"/>
+      <c r="C287" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D287" s="8"/>
     </row>
     <row r="288" ht="21" spans="1:4">
       <c r="A288" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B288" s="13" t="s">
+      <c r="B288" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C288" s="18"/>
+      <c r="C288" s="14"/>
       <c r="D288" s="8"/>
     </row>
     <row r="289" ht="21" spans="1:4">
       <c r="A289" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B289" s="13" t="s">
+      <c r="B289" s="10" t="s">
         <v>416</v>
       </c>
       <c r="C289" s="18"/>
@@ -6245,7 +6257,7 @@
       <c r="A290" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B290" s="13" t="s">
+      <c r="B290" s="10" t="s">
         <v>417</v>
       </c>
       <c r="C290" s="18"/>
@@ -6255,30 +6267,34 @@
       <c r="A291" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B291" s="13" t="s">
+      <c r="B291" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="C291" s="18"/>
+      <c r="C291" s="14"/>
       <c r="D291" s="8"/>
     </row>
     <row r="292" ht="21" spans="1:4">
       <c r="A292" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B292" s="13" t="s">
+      <c r="B292" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="C292" s="18"/>
+      <c r="C292" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D292" s="8"/>
     </row>
     <row r="293" ht="21" spans="1:4">
       <c r="A293" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B293" s="13" t="s">
+      <c r="B293" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="C293" s="18"/>
+      <c r="C293" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D293" s="8"/>
     </row>
     <row r="294" ht="21" spans="2:4">

</xml_diff>

<commit_message>
Stacks & Queues: Solved 11 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="C293" sqref="C293"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6311,10 +6311,10 @@
       <c r="A296" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B296" s="13" t="s">
+      <c r="B296" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="C296" s="18"/>
+      <c r="C296" s="17"/>
       <c r="D296" s="8"/>
     </row>
     <row r="297" ht="21" spans="1:4">
@@ -6324,27 +6324,27 @@
       <c r="B297" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="C297" s="18"/>
+      <c r="C297" s="17"/>
       <c r="D297" s="8"/>
     </row>
     <row r="298" ht="21" spans="1:4">
       <c r="A298" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B298" s="13" t="s">
+      <c r="B298" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C298" s="18"/>
+      <c r="C298" s="14"/>
       <c r="D298" s="8"/>
     </row>
     <row r="299" ht="21" spans="1:4">
       <c r="A299" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B299" s="13" t="s">
+      <c r="B299" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="C299" s="18"/>
+      <c r="C299" s="14"/>
       <c r="D299" s="8"/>
     </row>
     <row r="300" ht="21" spans="1:4">
@@ -6361,27 +6361,27 @@
       <c r="A301" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B301" s="13" t="s">
+      <c r="B301" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="C301" s="18"/>
+      <c r="C301" s="14"/>
       <c r="D301" s="8"/>
     </row>
     <row r="302" ht="21" spans="1:4">
       <c r="A302" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B302" s="13" t="s">
+      <c r="B302" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="C302" s="18"/>
+      <c r="C302" s="14"/>
       <c r="D302" s="8"/>
     </row>
     <row r="303" ht="21" spans="1:4">
       <c r="A303" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B303" s="13" t="s">
+      <c r="B303" s="10" t="s">
         <v>429</v>
       </c>
       <c r="C303" s="18"/>
@@ -6391,70 +6391,78 @@
       <c r="A304" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B304" s="13" t="s">
+      <c r="B304" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="C304" s="18"/>
+      <c r="C304" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D304" s="8"/>
     </row>
     <row r="305" ht="21" spans="1:4">
       <c r="A305" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B305" s="13" t="s">
+      <c r="B305" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C305" s="18"/>
+      <c r="C305" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D305" s="8"/>
     </row>
     <row r="306" ht="21" spans="1:4">
       <c r="A306" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B306" s="13" t="s">
+      <c r="B306" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C306" s="18"/>
+      <c r="C306" s="17"/>
       <c r="D306" s="8"/>
     </row>
     <row r="307" ht="21" spans="1:4">
       <c r="A307" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B307" s="13" t="s">
+      <c r="B307" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="C307" s="18"/>
+      <c r="C307" s="14"/>
       <c r="D307" s="8"/>
     </row>
     <row r="308" ht="21" spans="1:4">
       <c r="A308" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B308" s="13" t="s">
+      <c r="B308" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="C308" s="18"/>
+      <c r="C308" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D308" s="8"/>
     </row>
     <row r="309" ht="21" spans="1:4">
       <c r="A309" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B309" s="20" t="s">
+      <c r="B309" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="C309" s="18"/>
+      <c r="C309" s="14"/>
       <c r="D309" s="8"/>
     </row>
     <row r="310" ht="21" spans="1:4">
       <c r="A310" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B310" s="13" t="s">
+      <c r="B310" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="C310" s="18"/>
+      <c r="C310" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D310" s="8"/>
     </row>
     <row r="311" ht="21" spans="1:4">
@@ -6471,10 +6479,12 @@
       <c r="A312" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B312" s="13" t="s">
+      <c r="B312" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="C312" s="14"/>
+      <c r="C312" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D312" s="8"/>
     </row>
     <row r="313" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[COMPLETE]Stacks & Queues: Solved 14 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1881,9 +1881,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1972,6 +1972,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1980,8 +2041,29 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1996,48 +2078,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2050,59 +2094,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2153,7 +2153,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2165,49 +2183,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2225,19 +2207,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2261,7 +2237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2273,7 +2249,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2285,7 +2291,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2297,43 +2303,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2375,36 +2375,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2429,16 +2399,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2458,8 +2428,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2467,150 +2452,165 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="C310" sqref="C310"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6472,7 +6472,7 @@
       <c r="B311" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="C311" s="18"/>
+      <c r="C311" s="14"/>
       <c r="D311" s="8"/>
     </row>
     <row r="312" ht="21" spans="1:4">
@@ -6491,30 +6491,34 @@
       <c r="A313" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B313" s="13" t="s">
+      <c r="B313" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="C313" s="18"/>
+      <c r="C313" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D313" s="8"/>
     </row>
     <row r="314" ht="21" spans="1:4">
       <c r="A314" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B314" s="13" t="s">
+      <c r="B314" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="C314" s="18"/>
+      <c r="C314" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D314" s="8"/>
     </row>
     <row r="315" ht="21" spans="1:4">
       <c r="A315" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B315" s="13" t="s">
+      <c r="B315" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="C315" s="18"/>
+      <c r="C315" s="14"/>
       <c r="D315" s="8"/>
     </row>
     <row r="316" ht="21" spans="1:4">
@@ -6524,14 +6528,14 @@
       <c r="B316" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="C316" s="18"/>
+      <c r="C316" s="14"/>
       <c r="D316" s="8"/>
     </row>
     <row r="317" ht="21" spans="1:4">
       <c r="A317" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B317" s="13" t="s">
+      <c r="B317" s="10" t="s">
         <v>443</v>
       </c>
       <c r="C317" s="18"/>
@@ -6584,54 +6588,58 @@
       <c r="B322" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="C322" s="18"/>
+      <c r="C322" s="14"/>
       <c r="D322" s="8"/>
     </row>
     <row r="323" ht="21" spans="1:4">
       <c r="A323" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B323" s="13" t="s">
+      <c r="B323" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="C323" s="18"/>
+      <c r="C323" s="14"/>
       <c r="D323" s="8"/>
     </row>
     <row r="324" ht="21" spans="1:4">
       <c r="A324" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B324" s="13" t="s">
+      <c r="B324" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="C324" s="18"/>
+      <c r="C324" s="14"/>
       <c r="D324" s="8"/>
     </row>
     <row r="325" ht="21" spans="1:4">
       <c r="A325" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B325" s="13" t="s">
+      <c r="B325" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="C325" s="18"/>
+      <c r="C325" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D325" s="8"/>
     </row>
     <row r="326" ht="21" spans="1:4">
       <c r="A326" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B326" s="13" t="s">
+      <c r="B326" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C326" s="18"/>
+      <c r="C326" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D326" s="8"/>
     </row>
     <row r="327" ht="21" spans="1:4">
       <c r="A327" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B327" s="13" t="s">
+      <c r="B327" s="10" t="s">
         <v>453</v>
       </c>
       <c r="C327" s="18"/>
@@ -6641,10 +6649,10 @@
       <c r="A328" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B328" s="13" t="s">
+      <c r="B328" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="C328" s="18"/>
+      <c r="C328" s="14"/>
       <c r="D328" s="8"/>
     </row>
     <row r="329" ht="21" spans="1:4">
@@ -6661,40 +6669,44 @@
       <c r="A330" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B330" s="13" t="s">
+      <c r="B330" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="C330" s="18"/>
+      <c r="C330" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D330" s="8"/>
     </row>
     <row r="331" ht="21" spans="1:4">
       <c r="A331" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B331" s="13" t="s">
+      <c r="B331" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="C331" s="18"/>
+      <c r="C331" s="14"/>
       <c r="D331" s="8"/>
     </row>
     <row r="332" ht="21" spans="1:4">
       <c r="A332" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B332" s="13" t="s">
+      <c r="B332" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="C332" s="18"/>
+      <c r="C332" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D332" s="8"/>
     </row>
     <row r="333" ht="21" spans="1:4">
       <c r="A333" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B333" s="13" t="s">
+      <c r="B333" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="C333" s="18"/>
+      <c r="C333" s="14"/>
       <c r="D333" s="8"/>
     </row>
     <row r="334" ht="21" spans="2:4">

</xml_diff>

<commit_message>
[COMPLETE]Heaps: Solved 8 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="600">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1880,10 +1880,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1972,53 +1972,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2034,44 +1996,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2085,9 +2010,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2102,7 +2102,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2153,7 +2153,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2165,31 +2297,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2201,139 +2333,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2384,17 +2384,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2435,25 +2444,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2475,142 +2475,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2618,7 +2618,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2661,9 +2661,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2987,8 +2984,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="C353" sqref="C353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6575,7 +6572,7 @@
       <c r="A321" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B321" s="13" t="s">
+      <c r="B321" s="10" t="s">
         <v>447</v>
       </c>
       <c r="C321" s="18"/>
@@ -6726,37 +6723,37 @@
       <c r="B336" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="C336" s="18"/>
+      <c r="C336" s="17"/>
       <c r="D336" s="8"/>
     </row>
     <row r="337" ht="21" spans="1:4">
       <c r="A337" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B337" s="13" t="s">
+      <c r="B337" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C337" s="18"/>
+      <c r="C337" s="17"/>
       <c r="D337" s="8"/>
     </row>
     <row r="338" ht="21" spans="1:4">
       <c r="A338" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B338" s="13" t="s">
+      <c r="B338" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="C338" s="18"/>
+      <c r="C338" s="14"/>
       <c r="D338" s="8"/>
     </row>
     <row r="339" ht="21" spans="1:4">
       <c r="A339" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B339" s="13" t="s">
+      <c r="B339" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="C339" s="18"/>
+      <c r="C339" s="14"/>
       <c r="D339" s="8"/>
     </row>
     <row r="340" ht="21" spans="1:4">
@@ -6766,27 +6763,31 @@
       <c r="B340" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="C340" s="18"/>
+      <c r="C340" s="14"/>
       <c r="D340" s="8"/>
     </row>
     <row r="341" ht="21" spans="1:4">
       <c r="A341" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B341" s="13" t="s">
+      <c r="B341" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="C341" s="18"/>
+      <c r="C341" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D341" s="8"/>
     </row>
     <row r="342" ht="21" spans="1:4">
       <c r="A342" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B342" s="13" t="s">
+      <c r="B342" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="C342" s="18"/>
+      <c r="C342" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D342" s="8"/>
     </row>
     <row r="343" ht="21" spans="1:4">
@@ -6803,60 +6804,68 @@
       <c r="A344" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B344" s="20" t="s">
+      <c r="B344" s="19" t="s">
         <v>469</v>
       </c>
-      <c r="C344" s="18"/>
+      <c r="C344" s="14"/>
       <c r="D344" s="8"/>
     </row>
     <row r="345" ht="21" spans="1:4">
       <c r="A345" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B345" s="13" t="s">
+      <c r="B345" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="C345" s="18"/>
+      <c r="C345" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D345" s="8"/>
     </row>
     <row r="346" ht="21" spans="1:4">
       <c r="A346" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B346" s="13" t="s">
+      <c r="B346" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="C346" s="18"/>
+      <c r="C346" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D346" s="8"/>
     </row>
     <row r="347" ht="21" spans="1:4">
       <c r="A347" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B347" s="13" t="s">
+      <c r="B347" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="C347" s="18"/>
+      <c r="C347" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D347" s="8"/>
     </row>
     <row r="348" ht="21" spans="1:4">
       <c r="A348" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B348" s="13" t="s">
+      <c r="B348" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="C348" s="18"/>
+      <c r="C348" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D348" s="8"/>
     </row>
     <row r="349" ht="21" spans="1:4">
       <c r="A349" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B349" s="13" t="s">
+      <c r="B349" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="C349" s="18"/>
+      <c r="C349" s="14"/>
       <c r="D349" s="8"/>
     </row>
     <row r="350" ht="21" spans="1:4">
@@ -6883,20 +6892,20 @@
       <c r="A352" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B352" s="13" t="s">
+      <c r="B352" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="C352" s="18"/>
+      <c r="C352" s="14"/>
       <c r="D352" s="8"/>
     </row>
     <row r="353" ht="21" spans="1:4">
       <c r="A353" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B353" s="13" t="s">
+      <c r="B353" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="C353" s="18"/>
+      <c r="C353" s="14"/>
       <c r="D353" s="8"/>
     </row>
     <row r="354" ht="21" spans="2:4">

</xml_diff>

<commit_message>
[GRAPHS]: Solved 13 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510"/>
+    <workbookView windowWidth="28800" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1560,6 +1560,9 @@
     <t>Find whether it is possible to finish all tasks or not from given dependencies</t>
   </si>
   <si>
+    <t>Cycle detection</t>
+  </si>
+  <si>
     <t>Find the no. of Isalnds</t>
   </si>
   <si>
@@ -1880,10 +1883,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1980,69 +1983,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2057,14 +1999,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2078,8 +2013,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2095,6 +2045,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2102,7 +2098,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2159,7 +2162,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2171,31 +2186,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2213,13 +2246,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2231,31 +2300,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2267,67 +2324,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2375,39 +2378,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2425,10 +2395,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2437,8 +2405,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2459,6 +2427,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2472,124 +2466,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2598,16 +2601,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2984,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="C372" sqref="C372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6925,7 +6928,7 @@
       <c r="B356" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="C356" s="18"/>
+      <c r="C356" s="17"/>
       <c r="D356" s="8"/>
     </row>
     <row r="357" ht="21" spans="1:4">
@@ -6935,7 +6938,7 @@
       <c r="B357" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="C357" s="18"/>
+      <c r="C357" s="17"/>
       <c r="D357" s="8"/>
     </row>
     <row r="358" ht="21" spans="1:4">
@@ -6945,17 +6948,17 @@
       <c r="B358" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="C358" s="18"/>
+      <c r="C358" s="17"/>
       <c r="D358" s="8"/>
     </row>
     <row r="359" ht="21" spans="1:4">
       <c r="A359" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B359" s="13" t="s">
+      <c r="B359" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C359" s="18"/>
+      <c r="C359" s="14"/>
       <c r="D359" s="8"/>
     </row>
     <row r="360" ht="21" spans="1:4">
@@ -6965,77 +6968,77 @@
       <c r="B360" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="C360" s="18"/>
+      <c r="C360" s="14"/>
       <c r="D360" s="8"/>
     </row>
     <row r="361" ht="21" spans="1:4">
       <c r="A361" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B361" s="13" t="s">
+      <c r="B361" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="C361" s="18"/>
+      <c r="C361" s="14"/>
       <c r="D361" s="8"/>
     </row>
     <row r="362" ht="21" spans="1:4">
       <c r="A362" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B362" s="13" t="s">
+      <c r="B362" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="C362" s="18"/>
+      <c r="C362" s="14"/>
       <c r="D362" s="8"/>
     </row>
     <row r="363" ht="21" spans="1:4">
       <c r="A363" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B363" s="13" t="s">
+      <c r="B363" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="C363" s="18"/>
+      <c r="C363" s="14"/>
       <c r="D363" s="8"/>
     </row>
     <row r="364" ht="21" spans="1:4">
       <c r="A364" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B364" s="13" t="s">
+      <c r="B364" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="C364" s="18"/>
+      <c r="C364" s="14"/>
       <c r="D364" s="8"/>
     </row>
     <row r="365" ht="21" spans="1:4">
       <c r="A365" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B365" s="13" t="s">
+      <c r="B365" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="C365" s="18"/>
+      <c r="C365" s="14"/>
       <c r="D365" s="8"/>
     </row>
     <row r="366" ht="21" spans="1:4">
       <c r="A366" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B366" s="13" t="s">
+      <c r="B366" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="C366" s="18"/>
+      <c r="C366" s="14"/>
       <c r="D366" s="8"/>
     </row>
     <row r="367" ht="21" spans="1:4">
       <c r="A367" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B367" s="13" t="s">
+      <c r="B367" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="C367" s="18"/>
+      <c r="C367" s="17"/>
       <c r="D367" s="8"/>
     </row>
     <row r="368" ht="21" spans="1:4">
@@ -7045,47 +7048,49 @@
       <c r="B368" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="C368" s="18"/>
+      <c r="C368" s="17"/>
       <c r="D368" s="8"/>
     </row>
     <row r="369" ht="21" spans="1:4">
       <c r="A369" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B369" s="13" t="s">
+      <c r="B369" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="C369" s="18"/>
+      <c r="C369" s="14"/>
       <c r="D369" s="8"/>
     </row>
     <row r="370" ht="21" spans="1:4">
       <c r="A370" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B370" s="13" t="s">
+      <c r="B370" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="C370" s="18"/>
+      <c r="C370" s="14" t="s">
+        <v>495</v>
+      </c>
       <c r="D370" s="8"/>
     </row>
     <row r="371" ht="21" spans="1:4">
       <c r="A371" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B371" s="13" t="s">
-        <v>495</v>
-      </c>
-      <c r="C371" s="18"/>
+      <c r="B371" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="C371" s="14"/>
       <c r="D371" s="8"/>
     </row>
     <row r="372" ht="21" spans="1:4">
       <c r="A372" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B372" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="C372" s="18"/>
+      <c r="B372" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="C372" s="14"/>
       <c r="D372" s="8"/>
     </row>
     <row r="373" ht="21" spans="1:4">
@@ -7093,7 +7098,7 @@
         <v>479</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C373" s="18"/>
       <c r="D373" s="8"/>
@@ -7103,9 +7108,9 @@
         <v>479</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="C374" s="18"/>
+        <v>499</v>
+      </c>
+      <c r="C374" s="14"/>
       <c r="D374" s="8"/>
     </row>
     <row r="375" ht="21" spans="1:4">
@@ -7113,7 +7118,7 @@
         <v>479</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C375" s="18"/>
       <c r="D375" s="8"/>
@@ -7123,7 +7128,7 @@
         <v>479</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C376" s="18"/>
       <c r="D376" s="8"/>
@@ -7133,7 +7138,7 @@
         <v>479</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C377" s="18"/>
       <c r="D377" s="8"/>
@@ -7143,7 +7148,7 @@
         <v>479</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C378" s="18"/>
       <c r="D378" s="8"/>
@@ -7153,7 +7158,7 @@
         <v>479</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C379" s="18"/>
       <c r="D379" s="8"/>
@@ -7163,7 +7168,7 @@
         <v>479</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C380" s="18"/>
       <c r="D380" s="8"/>
@@ -7173,7 +7178,7 @@
         <v>479</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C381" s="18"/>
       <c r="D381" s="8"/>
@@ -7183,7 +7188,7 @@
         <v>479</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C382" s="18"/>
       <c r="D382" s="8"/>
@@ -7193,7 +7198,7 @@
         <v>479</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C383" s="18"/>
       <c r="D383" s="8"/>
@@ -7203,7 +7208,7 @@
         <v>479</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C384" s="18"/>
       <c r="D384" s="8"/>
@@ -7213,7 +7218,7 @@
         <v>479</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C385" s="18"/>
       <c r="D385" s="8"/>
@@ -7223,7 +7228,7 @@
         <v>479</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C386" s="18"/>
       <c r="D386" s="8"/>
@@ -7233,7 +7238,7 @@
         <v>479</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C387" s="18"/>
       <c r="D387" s="8"/>
@@ -7243,7 +7248,7 @@
         <v>479</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C388" s="18"/>
       <c r="D388" s="8"/>
@@ -7253,7 +7258,7 @@
         <v>479</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C389" s="18"/>
       <c r="D389" s="8"/>
@@ -7263,7 +7268,7 @@
         <v>479</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C390" s="18"/>
       <c r="D390" s="8"/>
@@ -7273,7 +7278,7 @@
         <v>479</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C391" s="18"/>
       <c r="D391" s="8"/>
@@ -7283,7 +7288,7 @@
         <v>479</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C392" s="18"/>
       <c r="D392" s="8"/>
@@ -7293,7 +7298,7 @@
         <v>479</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C393" s="18"/>
       <c r="D393" s="8"/>
@@ -7303,7 +7308,7 @@
         <v>479</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C394" s="18"/>
       <c r="D394" s="8"/>
@@ -7313,7 +7318,7 @@
         <v>479</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C395" s="18"/>
       <c r="D395" s="8"/>
@@ -7323,7 +7328,7 @@
         <v>479</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C396" s="18"/>
       <c r="D396" s="8"/>
@@ -7333,7 +7338,7 @@
         <v>479</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C397" s="18"/>
       <c r="D397" s="8"/>
@@ -7343,7 +7348,7 @@
         <v>479</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C398" s="18"/>
       <c r="D398" s="8"/>
@@ -7353,7 +7358,7 @@
         <v>479</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C399" s="18"/>
       <c r="D399" s="8"/>
@@ -7370,37 +7375,37 @@
     </row>
     <row r="402" ht="21" spans="1:4">
       <c r="A402" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C402" s="18"/>
       <c r="D402" s="8"/>
     </row>
     <row r="403" ht="21" spans="1:4">
       <c r="A403" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C403" s="18"/>
       <c r="D403" s="8"/>
     </row>
     <row r="404" ht="21" spans="1:4">
       <c r="A404" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C404" s="18"/>
       <c r="D404" s="8"/>
     </row>
     <row r="405" ht="21" spans="1:4">
       <c r="A405" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>165</v>
@@ -7410,20 +7415,20 @@
     </row>
     <row r="406" ht="21" spans="1:4">
       <c r="A406" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C406" s="18"/>
       <c r="D406" s="8"/>
     </row>
     <row r="407" ht="21" spans="1:4">
       <c r="A407" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C407" s="18"/>
       <c r="D407" s="8"/>
@@ -7440,77 +7445,77 @@
     </row>
     <row r="410" ht="21" spans="1:4">
       <c r="A410" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C410" s="18"/>
       <c r="D410" s="8"/>
     </row>
     <row r="411" ht="21" spans="1:4">
       <c r="A411" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C411" s="18"/>
       <c r="D411" s="8"/>
     </row>
     <row r="412" ht="21" spans="1:4">
       <c r="A412" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C412" s="18"/>
       <c r="D412" s="8"/>
     </row>
     <row r="413" ht="21" spans="1:4">
       <c r="A413" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C413" s="18"/>
       <c r="D413" s="8"/>
     </row>
     <row r="414" ht="21" spans="1:4">
       <c r="A414" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C414" s="18"/>
       <c r="D414" s="8"/>
     </row>
     <row r="415" ht="21" spans="1:4">
       <c r="A415" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C415" s="18"/>
       <c r="D415" s="8"/>
     </row>
     <row r="416" ht="21" spans="1:4">
       <c r="A416" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C416" s="18"/>
       <c r="D416" s="8"/>
     </row>
     <row r="417" ht="21" spans="1:4">
       <c r="A417" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B417" s="13" t="s">
         <v>409</v>
@@ -7520,520 +7525,520 @@
     </row>
     <row r="418" ht="21" spans="1:4">
       <c r="A418" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C418" s="18"/>
       <c r="D418" s="8"/>
     </row>
     <row r="419" ht="21" spans="1:4">
       <c r="A419" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C419" s="18"/>
       <c r="D419" s="8"/>
     </row>
     <row r="420" ht="21" spans="1:4">
       <c r="A420" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C420" s="18"/>
       <c r="D420" s="8"/>
     </row>
     <row r="421" ht="21" spans="1:4">
       <c r="A421" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C421" s="18"/>
       <c r="D421" s="8"/>
     </row>
     <row r="422" ht="21" spans="1:4">
       <c r="A422" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C422" s="18"/>
       <c r="D422" s="8"/>
     </row>
     <row r="423" ht="21" spans="1:4">
       <c r="A423" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C423" s="18"/>
       <c r="D423" s="8"/>
     </row>
     <row r="424" ht="21" spans="1:4">
       <c r="A424" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C424" s="18"/>
       <c r="D424" s="8"/>
     </row>
     <row r="425" ht="21" spans="1:4">
       <c r="A425" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C425" s="18"/>
       <c r="D425" s="8"/>
     </row>
     <row r="426" ht="21" spans="1:4">
       <c r="A426" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C426" s="18"/>
       <c r="D426" s="8"/>
     </row>
     <row r="427" ht="21" spans="1:4">
       <c r="A427" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C427" s="18"/>
       <c r="D427" s="8"/>
     </row>
     <row r="428" ht="21" spans="1:4">
       <c r="A428" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C428" s="18"/>
       <c r="D428" s="8"/>
     </row>
     <row r="429" ht="21" spans="1:4">
       <c r="A429" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C429" s="18"/>
       <c r="D429" s="8"/>
     </row>
     <row r="430" ht="21" spans="1:4">
       <c r="A430" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C430" s="18"/>
       <c r="D430" s="8"/>
     </row>
     <row r="431" ht="21" spans="1:4">
       <c r="A431" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C431" s="18"/>
       <c r="D431" s="8"/>
     </row>
     <row r="432" ht="21" spans="1:4">
       <c r="A432" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C432" s="18"/>
       <c r="D432" s="8"/>
     </row>
     <row r="433" ht="21" spans="1:4">
       <c r="A433" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C433" s="18"/>
       <c r="D433" s="8"/>
     </row>
     <row r="434" ht="21" spans="1:4">
       <c r="A434" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C434" s="18"/>
       <c r="D434" s="8"/>
     </row>
     <row r="435" ht="21" spans="1:4">
       <c r="A435" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C435" s="18"/>
       <c r="D435" s="8"/>
     </row>
     <row r="436" ht="21" spans="1:4">
       <c r="A436" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C436" s="18"/>
       <c r="D436" s="8"/>
     </row>
     <row r="437" ht="21" spans="1:4">
       <c r="A437" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C437" s="18"/>
       <c r="D437" s="8"/>
     </row>
     <row r="438" ht="21" spans="1:4">
       <c r="A438" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C438" s="18"/>
       <c r="D438" s="8"/>
     </row>
     <row r="439" ht="21" spans="1:4">
       <c r="A439" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C439" s="18"/>
       <c r="D439" s="8"/>
     </row>
     <row r="440" ht="21" spans="1:4">
       <c r="A440" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C440" s="18"/>
       <c r="D440" s="8"/>
     </row>
     <row r="441" ht="21" spans="1:4">
       <c r="A441" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C441" s="18"/>
       <c r="D441" s="8"/>
     </row>
     <row r="442" ht="21" spans="1:4">
       <c r="A442" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C442" s="18"/>
       <c r="D442" s="8"/>
     </row>
     <row r="443" ht="21" spans="1:4">
       <c r="A443" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C443" s="18"/>
       <c r="D443" s="8"/>
     </row>
     <row r="444" ht="21" spans="1:4">
       <c r="A444" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C444" s="18"/>
       <c r="D444" s="8"/>
     </row>
     <row r="445" ht="21" spans="1:4">
       <c r="A445" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C445" s="18"/>
       <c r="D445" s="8"/>
     </row>
     <row r="446" ht="21" spans="1:4">
       <c r="A446" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C446" s="18"/>
       <c r="D446" s="8"/>
     </row>
     <row r="447" ht="21" spans="1:4">
       <c r="A447" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C447" s="18"/>
       <c r="D447" s="8"/>
     </row>
     <row r="448" ht="21" spans="1:4">
       <c r="A448" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C448" s="18"/>
       <c r="D448" s="8"/>
     </row>
     <row r="449" ht="21" spans="1:4">
       <c r="A449" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C449" s="18"/>
       <c r="D449" s="8"/>
     </row>
     <row r="450" ht="21" spans="1:4">
       <c r="A450" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C450" s="18"/>
       <c r="D450" s="8"/>
     </row>
     <row r="451" ht="21" spans="1:4">
       <c r="A451" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C451" s="18"/>
       <c r="D451" s="8"/>
     </row>
     <row r="452" ht="21" spans="1:4">
       <c r="A452" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C452" s="18"/>
       <c r="D452" s="8"/>
     </row>
     <row r="453" ht="21" spans="1:4">
       <c r="A453" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C453" s="18"/>
       <c r="D453" s="8"/>
     </row>
     <row r="454" ht="21" spans="1:4">
       <c r="A454" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C454" s="18"/>
       <c r="D454" s="8"/>
     </row>
     <row r="455" ht="21" spans="1:4">
       <c r="A455" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C455" s="18"/>
       <c r="D455" s="8"/>
     </row>
     <row r="456" ht="21" spans="1:4">
       <c r="A456" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C456" s="18"/>
       <c r="D456" s="8"/>
     </row>
     <row r="457" ht="21" spans="1:4">
       <c r="A457" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C457" s="18"/>
       <c r="D457" s="8"/>
     </row>
     <row r="458" ht="21" spans="1:4">
       <c r="A458" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C458" s="18"/>
       <c r="D458" s="8"/>
     </row>
     <row r="459" ht="21" spans="1:4">
       <c r="A459" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C459" s="18"/>
       <c r="D459" s="8"/>
     </row>
     <row r="460" ht="21" spans="1:4">
       <c r="A460" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C460" s="18"/>
       <c r="D460" s="8"/>
     </row>
     <row r="461" ht="21" spans="1:4">
       <c r="A461" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C461" s="18"/>
       <c r="D461" s="8"/>
     </row>
     <row r="462" ht="21" spans="1:4">
       <c r="A462" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C462" s="18"/>
       <c r="D462" s="8"/>
     </row>
     <row r="463" ht="21" spans="1:4">
       <c r="A463" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C463" s="18"/>
       <c r="D463" s="8"/>
     </row>
     <row r="464" ht="21" spans="1:4">
       <c r="A464" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C464" s="18"/>
       <c r="D464" s="8"/>
     </row>
     <row r="465" ht="21" spans="1:4">
       <c r="A465" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C465" s="18"/>
       <c r="D465" s="8"/>
     </row>
     <row r="466" ht="21" spans="1:4">
       <c r="A466" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C466" s="18"/>
       <c r="D466" s="8"/>
     </row>
     <row r="467" ht="21" spans="1:4">
       <c r="A467" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C467" s="18"/>
       <c r="D467" s="8"/>
     </row>
     <row r="468" ht="21" spans="1:4">
       <c r="A468" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C468" s="18"/>
       <c r="D468" s="8"/>
     </row>
     <row r="469" ht="21" spans="1:4">
       <c r="A469" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C469" s="18"/>
       <c r="D469" s="8"/>
@@ -8051,100 +8056,100 @@
     </row>
     <row r="472" ht="21" spans="1:4">
       <c r="A472" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C472" s="18"/>
       <c r="D472" s="8"/>
     </row>
     <row r="473" ht="21" spans="1:4">
       <c r="A473" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C473" s="18"/>
       <c r="D473" s="8"/>
     </row>
     <row r="474" ht="21" spans="1:4">
       <c r="A474" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C474" s="18"/>
       <c r="D474" s="8"/>
     </row>
     <row r="475" ht="21" spans="1:4">
       <c r="A475" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C475" s="18"/>
       <c r="D475" s="8"/>
     </row>
     <row r="476" ht="21" spans="1:4">
       <c r="A476" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C476" s="18"/>
       <c r="D476" s="8"/>
     </row>
     <row r="477" ht="21" spans="1:4">
       <c r="A477" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C477" s="18"/>
       <c r="D477" s="8"/>
     </row>
     <row r="478" ht="21" spans="1:4">
       <c r="A478" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C478" s="18"/>
       <c r="D478" s="8"/>
     </row>
     <row r="479" ht="21" spans="1:4">
       <c r="A479" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C479" s="18"/>
       <c r="D479" s="8"/>
     </row>
     <row r="480" ht="21" spans="1:4">
       <c r="A480" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C480" s="18"/>
       <c r="D480" s="8"/>
     </row>
     <row r="481" ht="21" spans="1:4">
       <c r="A481" s="9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C481" s="18"/>
       <c r="D481" s="8"/>

</xml_diff>

<commit_message>
[GRAPHS]: Solved 11 questions.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12525"/>
+    <workbookView windowWidth="28800" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1602,7 +1602,7 @@
     <t>Check whether a graph is Bipartite or Not</t>
   </si>
   <si>
-    <t>Detect Negative cycle in a graph</t>
+    <t>Detect Negative cycle in a graph (Bellman ford)</t>
   </si>
   <si>
     <t>Longest path in a Directed Acyclic Graph</t>
@@ -1884,9 +1884,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1976,15 +1976,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1998,10 +2005,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2013,18 +2021,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2045,7 +2046,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2053,14 +2054,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2074,14 +2067,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -2089,9 +2074,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2106,6 +2090,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2156,25 +2156,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2192,18 +2198,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2216,7 +2210,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2228,55 +2300,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2288,43 +2312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2336,7 +2324,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2378,21 +2378,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2407,47 +2392,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2469,151 +2413,207 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2985,10 +2985,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D481"/>
+  <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="C372" sqref="C372"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="C392" sqref="C392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7100,7 +7100,7 @@
       <c r="B373" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="C373" s="18"/>
+      <c r="C373" s="14"/>
       <c r="D373" s="8"/>
     </row>
     <row r="374" ht="21" spans="1:4">
@@ -7117,47 +7117,47 @@
       <c r="A375" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B375" s="13" t="s">
+      <c r="B375" s="10" t="s">
         <v>500</v>
       </c>
-      <c r="C375" s="18"/>
+      <c r="C375" s="14"/>
       <c r="D375" s="8"/>
     </row>
     <row r="376" ht="21" spans="1:4">
       <c r="A376" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B376" s="13" t="s">
+      <c r="B376" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="C376" s="18"/>
+      <c r="C376" s="14"/>
       <c r="D376" s="8"/>
     </row>
     <row r="377" ht="21" spans="1:4">
       <c r="A377" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B377" s="13" t="s">
+      <c r="B377" s="10" t="s">
         <v>502</v>
       </c>
-      <c r="C377" s="18"/>
+      <c r="C377" s="14"/>
       <c r="D377" s="8"/>
     </row>
     <row r="378" ht="21" spans="1:4">
       <c r="A378" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B378" s="13" t="s">
+      <c r="B378" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="C378" s="18"/>
+      <c r="C378" s="14"/>
       <c r="D378" s="8"/>
     </row>
     <row r="379" ht="21" spans="1:4">
       <c r="A379" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B379" s="13" t="s">
+      <c r="B379" s="10" t="s">
         <v>504</v>
       </c>
       <c r="C379" s="18"/>
@@ -7167,20 +7167,20 @@
       <c r="A380" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B380" s="13" t="s">
+      <c r="B380" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="C380" s="18"/>
+      <c r="C380" s="14"/>
       <c r="D380" s="8"/>
     </row>
     <row r="381" ht="21" spans="1:4">
       <c r="A381" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B381" s="13" t="s">
+      <c r="B381" s="10" t="s">
         <v>506</v>
       </c>
-      <c r="C381" s="18"/>
+      <c r="C381" s="14"/>
       <c r="D381" s="8"/>
     </row>
     <row r="382" ht="21" spans="1:4">
@@ -7197,10 +7197,10 @@
       <c r="A383" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B383" s="13" t="s">
+      <c r="B383" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="C383" s="18"/>
+      <c r="C383" s="14"/>
       <c r="D383" s="8"/>
     </row>
     <row r="384" ht="21" spans="1:4">
@@ -7210,14 +7210,14 @@
       <c r="B384" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="C384" s="18"/>
+      <c r="C384" s="14"/>
       <c r="D384" s="8"/>
     </row>
     <row r="385" ht="21" spans="1:4">
       <c r="A385" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B385" s="13" t="s">
+      <c r="B385" s="10" t="s">
         <v>510</v>
       </c>
       <c r="C385" s="18"/>
@@ -7227,30 +7227,30 @@
       <c r="A386" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B386" s="13" t="s">
+      <c r="B386" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="C386" s="18"/>
+      <c r="C386" s="14"/>
       <c r="D386" s="8"/>
     </row>
     <row r="387" ht="21" spans="1:4">
       <c r="A387" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B387" s="13" t="s">
+      <c r="B387" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="C387" s="18"/>
+      <c r="C387" s="14"/>
       <c r="D387" s="8"/>
     </row>
     <row r="388" ht="21" spans="1:4">
       <c r="A388" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B388" s="13" t="s">
+      <c r="B388" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="C388" s="18"/>
+      <c r="C388" s="14"/>
       <c r="D388" s="8"/>
     </row>
     <row r="389" ht="21" spans="1:4">
@@ -7267,8 +7267,8 @@
       <c r="A390" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B390" s="13" t="s">
-        <v>514</v>
+      <c r="B390" s="10" t="s">
+        <v>515</v>
       </c>
       <c r="C390" s="18"/>
       <c r="D390" s="8"/>
@@ -7277,20 +7277,22 @@
       <c r="A391" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B391" s="13" t="s">
-        <v>515</v>
-      </c>
-      <c r="C391" s="18"/>
+      <c r="B391" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="C391" s="14"/>
       <c r="D391" s="8"/>
     </row>
     <row r="392" ht="21" spans="1:4">
       <c r="A392" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B392" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="C392" s="18"/>
+      <c r="B392" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="C392" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D392" s="8"/>
     </row>
     <row r="393" ht="21" spans="1:4">
@@ -7298,7 +7300,7 @@
         <v>479</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C393" s="18"/>
       <c r="D393" s="8"/>
@@ -7308,7 +7310,7 @@
         <v>479</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C394" s="18"/>
       <c r="D394" s="8"/>
@@ -7318,7 +7320,7 @@
         <v>479</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C395" s="18"/>
       <c r="D395" s="8"/>
@@ -7328,7 +7330,7 @@
         <v>479</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C396" s="18"/>
       <c r="D396" s="8"/>
@@ -7338,7 +7340,7 @@
         <v>479</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C397" s="18"/>
       <c r="D397" s="8"/>
@@ -7348,19 +7350,14 @@
         <v>479</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C398" s="18"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" ht="21" spans="1:4">
-      <c r="A399" s="16" t="s">
-        <v>479</v>
-      </c>
-      <c r="B399" s="13" t="s">
-        <v>523</v>
-      </c>
-      <c r="C399" s="18"/>
+    <row r="399" ht="21" spans="2:4">
+      <c r="B399" s="8"/>
+      <c r="C399" s="15"/>
       <c r="D399" s="8"/>
     </row>
     <row r="400" ht="21" spans="2:4">
@@ -7368,9 +7365,14 @@
       <c r="C400" s="15"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" ht="21" spans="2:4">
-      <c r="B401" s="8"/>
-      <c r="C401" s="15"/>
+    <row r="401" ht="21" spans="1:4">
+      <c r="A401" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B401" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="C401" s="18"/>
       <c r="D401" s="8"/>
     </row>
     <row r="402" ht="21" spans="1:4">
@@ -7378,7 +7380,7 @@
         <v>524</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C402" s="18"/>
       <c r="D402" s="8"/>
@@ -7388,7 +7390,7 @@
         <v>524</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C403" s="18"/>
       <c r="D403" s="8"/>
@@ -7398,7 +7400,7 @@
         <v>524</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>527</v>
+        <v>165</v>
       </c>
       <c r="C404" s="18"/>
       <c r="D404" s="8"/>
@@ -7408,7 +7410,7 @@
         <v>524</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>165</v>
+        <v>528</v>
       </c>
       <c r="C405" s="18"/>
       <c r="D405" s="8"/>
@@ -7418,19 +7420,14 @@
         <v>524</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C406" s="18"/>
       <c r="D406" s="8"/>
     </row>
-    <row r="407" ht="21" spans="1:4">
-      <c r="A407" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="B407" s="13" t="s">
-        <v>529</v>
-      </c>
-      <c r="C407" s="18"/>
+    <row r="407" ht="21" spans="2:4">
+      <c r="B407" s="8"/>
+      <c r="C407" s="15"/>
       <c r="D407" s="8"/>
     </row>
     <row r="408" ht="21" spans="2:4">
@@ -7438,9 +7435,14 @@
       <c r="C408" s="15"/>
       <c r="D408" s="8"/>
     </row>
-    <row r="409" ht="21" spans="2:4">
-      <c r="B409" s="8"/>
-      <c r="C409" s="15"/>
+    <row r="409" ht="21" spans="1:4">
+      <c r="A409" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="B409" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="C409" s="18"/>
       <c r="D409" s="8"/>
     </row>
     <row r="410" ht="21" spans="1:4">
@@ -7448,7 +7450,7 @@
         <v>530</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C410" s="18"/>
       <c r="D410" s="8"/>
@@ -7458,7 +7460,7 @@
         <v>530</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C411" s="18"/>
       <c r="D411" s="8"/>
@@ -7468,7 +7470,7 @@
         <v>530</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C412" s="18"/>
       <c r="D412" s="8"/>
@@ -7478,7 +7480,7 @@
         <v>530</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C413" s="18"/>
       <c r="D413" s="8"/>
@@ -7488,7 +7490,7 @@
         <v>530</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C414" s="18"/>
       <c r="D414" s="8"/>
@@ -7498,7 +7500,7 @@
         <v>530</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C415" s="18"/>
       <c r="D415" s="8"/>
@@ -7508,7 +7510,7 @@
         <v>530</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>537</v>
+        <v>409</v>
       </c>
       <c r="C416" s="18"/>
       <c r="D416" s="8"/>
@@ -7518,7 +7520,7 @@
         <v>530</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>409</v>
+        <v>538</v>
       </c>
       <c r="C417" s="18"/>
       <c r="D417" s="8"/>
@@ -7528,7 +7530,7 @@
         <v>530</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C418" s="18"/>
       <c r="D418" s="8"/>
@@ -7538,7 +7540,7 @@
         <v>530</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C419" s="18"/>
       <c r="D419" s="8"/>
@@ -7548,7 +7550,7 @@
         <v>530</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C420" s="18"/>
       <c r="D420" s="8"/>
@@ -7558,7 +7560,7 @@
         <v>530</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C421" s="18"/>
       <c r="D421" s="8"/>
@@ -7568,7 +7570,7 @@
         <v>530</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C422" s="18"/>
       <c r="D422" s="8"/>
@@ -7578,7 +7580,7 @@
         <v>530</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C423" s="18"/>
       <c r="D423" s="8"/>
@@ -7588,7 +7590,7 @@
         <v>530</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C424" s="18"/>
       <c r="D424" s="8"/>
@@ -7598,7 +7600,7 @@
         <v>530</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C425" s="18"/>
       <c r="D425" s="8"/>
@@ -7608,7 +7610,7 @@
         <v>530</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C426" s="18"/>
       <c r="D426" s="8"/>
@@ -7618,7 +7620,7 @@
         <v>530</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C427" s="18"/>
       <c r="D427" s="8"/>
@@ -7628,7 +7630,7 @@
         <v>530</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C428" s="18"/>
       <c r="D428" s="8"/>
@@ -7638,7 +7640,7 @@
         <v>530</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C429" s="18"/>
       <c r="D429" s="8"/>
@@ -7648,7 +7650,7 @@
         <v>530</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C430" s="18"/>
       <c r="D430" s="8"/>
@@ -7658,7 +7660,7 @@
         <v>530</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C431" s="18"/>
       <c r="D431" s="8"/>
@@ -7668,7 +7670,7 @@
         <v>530</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C432" s="18"/>
       <c r="D432" s="8"/>
@@ -7678,7 +7680,7 @@
         <v>530</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C433" s="18"/>
       <c r="D433" s="8"/>
@@ -7688,7 +7690,7 @@
         <v>530</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C434" s="18"/>
       <c r="D434" s="8"/>
@@ -7698,7 +7700,7 @@
         <v>530</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C435" s="18"/>
       <c r="D435" s="8"/>
@@ -7708,7 +7710,7 @@
         <v>530</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C436" s="18"/>
       <c r="D436" s="8"/>
@@ -7718,7 +7720,7 @@
         <v>530</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C437" s="18"/>
       <c r="D437" s="8"/>
@@ -7728,7 +7730,7 @@
         <v>530</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C438" s="18"/>
       <c r="D438" s="8"/>
@@ -7738,7 +7740,7 @@
         <v>530</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C439" s="18"/>
       <c r="D439" s="8"/>
@@ -7748,7 +7750,7 @@
         <v>530</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C440" s="18"/>
       <c r="D440" s="8"/>
@@ -7758,7 +7760,7 @@
         <v>530</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C441" s="18"/>
       <c r="D441" s="8"/>
@@ -7768,7 +7770,7 @@
         <v>530</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C442" s="18"/>
       <c r="D442" s="8"/>
@@ -7778,7 +7780,7 @@
         <v>530</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C443" s="18"/>
       <c r="D443" s="8"/>
@@ -7788,7 +7790,7 @@
         <v>530</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C444" s="18"/>
       <c r="D444" s="8"/>
@@ -7798,7 +7800,7 @@
         <v>530</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C445" s="18"/>
       <c r="D445" s="8"/>
@@ -7808,7 +7810,7 @@
         <v>530</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C446" s="18"/>
       <c r="D446" s="8"/>
@@ -7818,7 +7820,7 @@
         <v>530</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C447" s="18"/>
       <c r="D447" s="8"/>
@@ -7828,7 +7830,7 @@
         <v>530</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C448" s="18"/>
       <c r="D448" s="8"/>
@@ -7838,7 +7840,7 @@
         <v>530</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C449" s="18"/>
       <c r="D449" s="8"/>
@@ -7848,7 +7850,7 @@
         <v>530</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C450" s="18"/>
       <c r="D450" s="8"/>
@@ -7858,7 +7860,7 @@
         <v>530</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C451" s="18"/>
       <c r="D451" s="8"/>
@@ -7868,7 +7870,7 @@
         <v>530</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C452" s="18"/>
       <c r="D452" s="8"/>
@@ -7878,7 +7880,7 @@
         <v>530</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C453" s="18"/>
       <c r="D453" s="8"/>
@@ -7888,7 +7890,7 @@
         <v>530</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C454" s="18"/>
       <c r="D454" s="8"/>
@@ -7898,7 +7900,7 @@
         <v>530</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C455" s="18"/>
       <c r="D455" s="8"/>
@@ -7908,7 +7910,7 @@
         <v>530</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C456" s="18"/>
       <c r="D456" s="8"/>
@@ -7918,7 +7920,7 @@
         <v>530</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C457" s="18"/>
       <c r="D457" s="8"/>
@@ -7928,7 +7930,7 @@
         <v>530</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C458" s="18"/>
       <c r="D458" s="8"/>
@@ -7938,7 +7940,7 @@
         <v>530</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C459" s="18"/>
       <c r="D459" s="8"/>
@@ -7948,7 +7950,7 @@
         <v>530</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C460" s="18"/>
       <c r="D460" s="8"/>
@@ -7958,7 +7960,7 @@
         <v>530</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C461" s="18"/>
       <c r="D461" s="8"/>
@@ -7968,7 +7970,7 @@
         <v>530</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C462" s="18"/>
       <c r="D462" s="8"/>
@@ -7978,7 +7980,7 @@
         <v>530</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C463" s="18"/>
       <c r="D463" s="8"/>
@@ -7988,7 +7990,7 @@
         <v>530</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C464" s="18"/>
       <c r="D464" s="8"/>
@@ -7998,7 +8000,7 @@
         <v>530</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C465" s="18"/>
       <c r="D465" s="8"/>
@@ -8008,7 +8010,7 @@
         <v>530</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C466" s="18"/>
       <c r="D466" s="8"/>
@@ -8018,7 +8020,7 @@
         <v>530</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C467" s="18"/>
       <c r="D467" s="8"/>
@@ -8028,30 +8030,30 @@
         <v>530</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C468" s="18"/>
       <c r="D468" s="8"/>
     </row>
-    <row r="469" ht="21" spans="1:4">
-      <c r="A469" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="B469" s="13" t="s">
-        <v>589</v>
-      </c>
-      <c r="C469" s="18"/>
+    <row r="469" ht="21" spans="2:4">
+      <c r="B469" s="8"/>
+      <c r="C469" s="15"/>
       <c r="D469" s="8"/>
     </row>
-    <row r="470" ht="21" spans="2:4">
+    <row r="470" ht="21" spans="1:4">
+      <c r="A470" s="16"/>
       <c r="B470" s="8"/>
       <c r="C470" s="15"/>
       <c r="D470" s="8"/>
     </row>
     <row r="471" ht="21" spans="1:4">
-      <c r="A471" s="16"/>
-      <c r="B471" s="8"/>
-      <c r="C471" s="15"/>
+      <c r="A471" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="B471" s="13" t="s">
+        <v>591</v>
+      </c>
+      <c r="C471" s="18"/>
       <c r="D471" s="8"/>
     </row>
     <row r="472" ht="21" spans="1:4">
@@ -8059,7 +8061,7 @@
         <v>590</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C472" s="18"/>
       <c r="D472" s="8"/>
@@ -8069,7 +8071,7 @@
         <v>590</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C473" s="18"/>
       <c r="D473" s="8"/>
@@ -8079,7 +8081,7 @@
         <v>590</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C474" s="18"/>
       <c r="D474" s="8"/>
@@ -8089,7 +8091,7 @@
         <v>590</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C475" s="18"/>
       <c r="D475" s="8"/>
@@ -8099,7 +8101,7 @@
         <v>590</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C476" s="18"/>
       <c r="D476" s="8"/>
@@ -8109,7 +8111,7 @@
         <v>590</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C477" s="18"/>
       <c r="D477" s="8"/>
@@ -8119,7 +8121,7 @@
         <v>590</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C478" s="18"/>
       <c r="D478" s="8"/>
@@ -8129,7 +8131,7 @@
         <v>590</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C479" s="18"/>
       <c r="D479" s="8"/>
@@ -8139,20 +8141,10 @@
         <v>590</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C480" s="18"/>
       <c r="D480" s="8"/>
-    </row>
-    <row r="481" ht="21" spans="1:4">
-      <c r="A481" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="B481" s="13" t="s">
-        <v>600</v>
-      </c>
-      <c r="C481" s="18"/>
-      <c r="D481" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8506,98 +8498,97 @@
     <hyperlink ref="B381" r:id="rId335" display="Find bridge in a graph"/>
     <hyperlink ref="B382" r:id="rId336" display="Count Strongly connected Components(Kosaraju Algo)"/>
     <hyperlink ref="B383" r:id="rId337" display="Check whether a graph is Bipartite or Not"/>
-    <hyperlink ref="B384" r:id="rId338" display="Detect Negative cycle in a graph"/>
+    <hyperlink ref="B384" r:id="rId338" display="Detect Negative cycle in a graph (Bellman ford)"/>
     <hyperlink ref="B385" r:id="rId339" display="Longest path in a Directed Acyclic Graph"/>
     <hyperlink ref="B386" r:id="rId340" display="Journey to the Moon"/>
     <hyperlink ref="B387" r:id="rId341" display="Cheapest Flights Within K Stops"/>
     <hyperlink ref="B388" r:id="rId342" display="Oliver and the Game"/>
     <hyperlink ref="B389" r:id="rId343" display="Water Jug problem using BFS"/>
-    <hyperlink ref="B390" r:id="rId343" display="Water Jug problem using BFS"/>
-    <hyperlink ref="B391" r:id="rId256" display="Find if there is a path of more thank length from a source"/>
-    <hyperlink ref="B392" r:id="rId248" display="M-ColouringProblem"/>
-    <hyperlink ref="B393" r:id="rId344" display="Minimum edges to reverse o make path from source to destination"/>
-    <hyperlink ref="B394" r:id="rId345" display="Paths to travel each nodes using each edge(Seven Bridges)"/>
-    <hyperlink ref="B396" r:id="rId346" display="Chinese Postman or Route Inspection"/>
-    <hyperlink ref="B395" r:id="rId347" display="Vertex Cover Problem"/>
-    <hyperlink ref="B397" r:id="rId348" display="Number of Triangles in a Directed and Undirected Graph"/>
-    <hyperlink ref="B398" r:id="rId220" display="Minimise the cashflow among a given set of friends who have borrowed money from each other"/>
-    <hyperlink ref="B399" r:id="rId349" display="Two Clique Problem"/>
-    <hyperlink ref="B402" r:id="rId350" display="Construct a trie from scratch"/>
-    <hyperlink ref="B403" r:id="rId351" display="Find shortest unique prefix for every word in a given list"/>
-    <hyperlink ref="B404" r:id="rId352" display="Word Break Problem | (Trie solution)"/>
-    <hyperlink ref="B405" r:id="rId78" display="Given a sequence of words, print all anagrams together"/>
-    <hyperlink ref="B406" r:id="rId353" display="Implement a Phone Directory"/>
-    <hyperlink ref="B407" r:id="rId354" display="Print unique rows in a given boolean matrix"/>
-    <hyperlink ref="B410" r:id="rId355" display="Coin ChangeProblem"/>
-    <hyperlink ref="B411" r:id="rId356" display="Knapsack Problem"/>
-    <hyperlink ref="B412" r:id="rId357" display="Binomial CoefficientProblem"/>
-    <hyperlink ref="B413" r:id="rId358" display="Permutation CoefficientProblem"/>
-    <hyperlink ref="B414" r:id="rId359" display="Program for nth Catalan Number"/>
-    <hyperlink ref="B415" r:id="rId360" display="Matrix Chain Multiplication "/>
-    <hyperlink ref="B416" r:id="rId56" display="Edit Distance"/>
-    <hyperlink ref="B417" r:id="rId250" display="Subset Sum Problem"/>
-    <hyperlink ref="B418" r:id="rId361" display="Friends Pairing Problem"/>
-    <hyperlink ref="B419" r:id="rId362" display="Gold Mine Problem"/>
-    <hyperlink ref="B420" r:id="rId363" display="Assembly Line SchedulingProblem"/>
-    <hyperlink ref="B421" r:id="rId364" display="Painting the Fenceproblem"/>
-    <hyperlink ref="B422" r:id="rId365" display="Maximize The Cut Segments"/>
-    <hyperlink ref="B423" r:id="rId73" display="Longest Common Subsequence"/>
-    <hyperlink ref="B424" r:id="rId52" display="Longest Repeated Subsequence"/>
-    <hyperlink ref="B425" r:id="rId366" display="Longest Increasing Subsequence"/>
-    <hyperlink ref="B426" r:id="rId367" display="Space Optimized Solution of LCS"/>
-    <hyperlink ref="B427" r:id="rId368" display="LCS (Longest Common Subsequence) of three strings"/>
-    <hyperlink ref="B428" r:id="rId369" display="Maximum Sum Increasing Subsequence"/>
-    <hyperlink ref="B429" r:id="rId370" display="Count all subsequences having product less than K"/>
-    <hyperlink ref="B430" r:id="rId371" display="Longest subsequence such that difference between adjacent is one"/>
-    <hyperlink ref="B431" r:id="rId372" display="Maximum subsequence sum such that no three are consecutive"/>
-    <hyperlink ref="B432" r:id="rId373" display="Egg Dropping Problem"/>
-    <hyperlink ref="B433" r:id="rId374" display="Maximum Length Chain of Pairs"/>
-    <hyperlink ref="B434" r:id="rId375" display="Maximum size square sub-matrix with all 1s"/>
-    <hyperlink ref="B435" r:id="rId376" display="Maximum sum of pairs with specific difference"/>
-    <hyperlink ref="B436" r:id="rId377" display="Min Cost PathProblem"/>
-    <hyperlink ref="B437" r:id="rId378" display="Maximum difference of zeros and ones in binary string"/>
-    <hyperlink ref="B438" r:id="rId10" display="Minimum number of jumps to reach end"/>
-    <hyperlink ref="B439" r:id="rId379" display="Minimum cost to fill given weight in a bag"/>
-    <hyperlink ref="B440" r:id="rId380" display="Minimum removals from array to make max –min &lt;= K"/>
-    <hyperlink ref="B441" r:id="rId381" display="Longest Common Substring"/>
-    <hyperlink ref="B442" r:id="rId382" display="Count number of ways to reacha given score in a game"/>
-    <hyperlink ref="B443" r:id="rId383" display="Count Balanced Binary Trees of Height h"/>
-    <hyperlink ref="B444" r:id="rId8" display="LargestSum Contiguous Subarray [V&gt;V&gt;V&gt;V IMP ]"/>
-    <hyperlink ref="B445" r:id="rId384" display="Smallest sum contiguous subarray"/>
-    <hyperlink ref="B446" r:id="rId385" display="Unbounded Knapsack (Repetition of items allowed)"/>
-    <hyperlink ref="B447" r:id="rId59" display="Word Break Problem"/>
-    <hyperlink ref="B448" r:id="rId386" display="Largest Independent Set Problem"/>
-    <hyperlink ref="B449" r:id="rId250" display="Partition problem"/>
-    <hyperlink ref="B451" r:id="rId64" display="Count All Palindromic Subsequence in a given String"/>
-    <hyperlink ref="B450" r:id="rId387" display="Longest Palindromic Subsequence"/>
-    <hyperlink ref="B452" r:id="rId388" display="Longest Palindromic Substring"/>
-    <hyperlink ref="B453" r:id="rId389" display="Longest alternating subsequence"/>
-    <hyperlink ref="B454" r:id="rId390" display="Weighted Job Scheduling"/>
-    <hyperlink ref="B455" r:id="rId391" display="Coin game winner where every player has three choices"/>
-    <hyperlink ref="B456" r:id="rId392" display="Count Derangements (Permutation such that no element appears in its original position) [ IMP ]"/>
-    <hyperlink ref="B457" r:id="rId25" display="Maximum profit by buying and selling a share at most twice [ IMP ]"/>
-    <hyperlink ref="B458" r:id="rId393" display="Optimal Strategy for a Game"/>
-    <hyperlink ref="B459" r:id="rId394" display="Optimal Binary Search Tree"/>
-    <hyperlink ref="B460" r:id="rId395" display="Palindrome PartitioningProblem"/>
-    <hyperlink ref="B461" r:id="rId55" display="Word Wrap Problem"/>
-    <hyperlink ref="B462" r:id="rId396" display="Mobile Numeric Keypad Problem [ IMP ]"/>
-    <hyperlink ref="B469" r:id="rId397" display="Maximum Length of Pair Chain"/>
-    <hyperlink ref="B468" r:id="rId398" display="Find if a string is interleaved of two other strings"/>
-    <hyperlink ref="B467" r:id="rId399" display="Maximum profit by buying and selling a share at most k times"/>
-    <hyperlink ref="B466" r:id="rId400" display="Maximum sum rectangle in a 2D matrix"/>
-    <hyperlink ref="B465" r:id="rId401" display="Largest area rectangular sub-matrix with equal number of 1’s and 0’s [ IMP ]"/>
-    <hyperlink ref="B464" r:id="rId402" display="Largest rectangular sub-matrix whose sum is 0"/>
-    <hyperlink ref="B463" r:id="rId403" display="Boolean Parenthesization Problem"/>
-    <hyperlink ref="B472" r:id="rId404" display="Count set bits in an integer"/>
-    <hyperlink ref="B473" r:id="rId405" display="Find the two non-repeating elements in an array of repeating elements"/>
-    <hyperlink ref="B474" r:id="rId406" display="Count number of bits to be flipped to convert A to B"/>
-    <hyperlink ref="B475" r:id="rId407" display="Count total set bits in all numbers from 1 to n"/>
-    <hyperlink ref="B476" r:id="rId408" display="Program to find whether a no is power of two"/>
-    <hyperlink ref="B477" r:id="rId409" display="Find position of the only set bit"/>
-    <hyperlink ref="B478" r:id="rId410" display="Copy set bits in a range"/>
-    <hyperlink ref="B481" r:id="rId411" display="Power Set"/>
-    <hyperlink ref="B479" r:id="rId412" display="Divide two integers without using multiplication, division and mod operator"/>
-    <hyperlink ref="B480" r:id="rId413" display="Calculate square of a number without using *, / and pow()"/>
+    <hyperlink ref="B390" r:id="rId256" display="Find if there is a path of more thank length from a source"/>
+    <hyperlink ref="B391" r:id="rId248" display="M-ColouringProblem"/>
+    <hyperlink ref="B392" r:id="rId344" display="Minimum edges to reverse o make path from source to destination"/>
+    <hyperlink ref="B393" r:id="rId345" display="Paths to travel each nodes using each edge(Seven Bridges)"/>
+    <hyperlink ref="B395" r:id="rId346" display="Chinese Postman or Route Inspection"/>
+    <hyperlink ref="B394" r:id="rId347" display="Vertex Cover Problem"/>
+    <hyperlink ref="B396" r:id="rId348" display="Number of Triangles in a Directed and Undirected Graph"/>
+    <hyperlink ref="B397" r:id="rId220" display="Minimise the cashflow among a given set of friends who have borrowed money from each other"/>
+    <hyperlink ref="B398" r:id="rId349" display="Two Clique Problem"/>
+    <hyperlink ref="B401" r:id="rId350" display="Construct a trie from scratch"/>
+    <hyperlink ref="B402" r:id="rId351" display="Find shortest unique prefix for every word in a given list"/>
+    <hyperlink ref="B403" r:id="rId352" display="Word Break Problem | (Trie solution)"/>
+    <hyperlink ref="B404" r:id="rId78" display="Given a sequence of words, print all anagrams together"/>
+    <hyperlink ref="B405" r:id="rId353" display="Implement a Phone Directory"/>
+    <hyperlink ref="B406" r:id="rId354" display="Print unique rows in a given boolean matrix"/>
+    <hyperlink ref="B409" r:id="rId355" display="Coin ChangeProblem"/>
+    <hyperlink ref="B410" r:id="rId356" display="Knapsack Problem"/>
+    <hyperlink ref="B411" r:id="rId357" display="Binomial CoefficientProblem"/>
+    <hyperlink ref="B412" r:id="rId358" display="Permutation CoefficientProblem"/>
+    <hyperlink ref="B413" r:id="rId359" display="Program for nth Catalan Number"/>
+    <hyperlink ref="B414" r:id="rId360" display="Matrix Chain Multiplication "/>
+    <hyperlink ref="B415" r:id="rId56" display="Edit Distance"/>
+    <hyperlink ref="B416" r:id="rId250" display="Subset Sum Problem"/>
+    <hyperlink ref="B417" r:id="rId361" display="Friends Pairing Problem"/>
+    <hyperlink ref="B418" r:id="rId362" display="Gold Mine Problem"/>
+    <hyperlink ref="B419" r:id="rId363" display="Assembly Line SchedulingProblem"/>
+    <hyperlink ref="B420" r:id="rId364" display="Painting the Fenceproblem"/>
+    <hyperlink ref="B421" r:id="rId365" display="Maximize The Cut Segments"/>
+    <hyperlink ref="B422" r:id="rId73" display="Longest Common Subsequence"/>
+    <hyperlink ref="B423" r:id="rId52" display="Longest Repeated Subsequence"/>
+    <hyperlink ref="B424" r:id="rId366" display="Longest Increasing Subsequence"/>
+    <hyperlink ref="B425" r:id="rId367" display="Space Optimized Solution of LCS"/>
+    <hyperlink ref="B426" r:id="rId368" display="LCS (Longest Common Subsequence) of three strings"/>
+    <hyperlink ref="B427" r:id="rId369" display="Maximum Sum Increasing Subsequence"/>
+    <hyperlink ref="B428" r:id="rId370" display="Count all subsequences having product less than K"/>
+    <hyperlink ref="B429" r:id="rId371" display="Longest subsequence such that difference between adjacent is one"/>
+    <hyperlink ref="B430" r:id="rId372" display="Maximum subsequence sum such that no three are consecutive"/>
+    <hyperlink ref="B431" r:id="rId373" display="Egg Dropping Problem"/>
+    <hyperlink ref="B432" r:id="rId374" display="Maximum Length Chain of Pairs"/>
+    <hyperlink ref="B433" r:id="rId375" display="Maximum size square sub-matrix with all 1s"/>
+    <hyperlink ref="B434" r:id="rId376" display="Maximum sum of pairs with specific difference"/>
+    <hyperlink ref="B435" r:id="rId377" display="Min Cost PathProblem"/>
+    <hyperlink ref="B436" r:id="rId378" display="Maximum difference of zeros and ones in binary string"/>
+    <hyperlink ref="B437" r:id="rId10" display="Minimum number of jumps to reach end"/>
+    <hyperlink ref="B438" r:id="rId379" display="Minimum cost to fill given weight in a bag"/>
+    <hyperlink ref="B439" r:id="rId380" display="Minimum removals from array to make max –min &lt;= K"/>
+    <hyperlink ref="B440" r:id="rId381" display="Longest Common Substring"/>
+    <hyperlink ref="B441" r:id="rId382" display="Count number of ways to reacha given score in a game"/>
+    <hyperlink ref="B442" r:id="rId383" display="Count Balanced Binary Trees of Height h"/>
+    <hyperlink ref="B443" r:id="rId8" display="LargestSum Contiguous Subarray [V&gt;V&gt;V&gt;V IMP ]"/>
+    <hyperlink ref="B444" r:id="rId384" display="Smallest sum contiguous subarray"/>
+    <hyperlink ref="B445" r:id="rId385" display="Unbounded Knapsack (Repetition of items allowed)"/>
+    <hyperlink ref="B446" r:id="rId59" display="Word Break Problem"/>
+    <hyperlink ref="B447" r:id="rId386" display="Largest Independent Set Problem"/>
+    <hyperlink ref="B448" r:id="rId250" display="Partition problem"/>
+    <hyperlink ref="B450" r:id="rId64" display="Count All Palindromic Subsequence in a given String"/>
+    <hyperlink ref="B449" r:id="rId387" display="Longest Palindromic Subsequence"/>
+    <hyperlink ref="B451" r:id="rId388" display="Longest Palindromic Substring"/>
+    <hyperlink ref="B452" r:id="rId389" display="Longest alternating subsequence"/>
+    <hyperlink ref="B453" r:id="rId390" display="Weighted Job Scheduling"/>
+    <hyperlink ref="B454" r:id="rId391" display="Coin game winner where every player has three choices"/>
+    <hyperlink ref="B455" r:id="rId392" display="Count Derangements (Permutation such that no element appears in its original position) [ IMP ]"/>
+    <hyperlink ref="B456" r:id="rId25" display="Maximum profit by buying and selling a share at most twice [ IMP ]"/>
+    <hyperlink ref="B457" r:id="rId393" display="Optimal Strategy for a Game"/>
+    <hyperlink ref="B458" r:id="rId394" display="Optimal Binary Search Tree"/>
+    <hyperlink ref="B459" r:id="rId395" display="Palindrome PartitioningProblem"/>
+    <hyperlink ref="B460" r:id="rId55" display="Word Wrap Problem"/>
+    <hyperlink ref="B461" r:id="rId396" display="Mobile Numeric Keypad Problem [ IMP ]"/>
+    <hyperlink ref="B468" r:id="rId397" display="Maximum Length of Pair Chain"/>
+    <hyperlink ref="B467" r:id="rId398" display="Find if a string is interleaved of two other strings"/>
+    <hyperlink ref="B466" r:id="rId399" display="Maximum profit by buying and selling a share at most k times"/>
+    <hyperlink ref="B465" r:id="rId400" display="Maximum sum rectangle in a 2D matrix"/>
+    <hyperlink ref="B464" r:id="rId401" display="Largest area rectangular sub-matrix with equal number of 1’s and 0’s [ IMP ]"/>
+    <hyperlink ref="B463" r:id="rId402" display="Largest rectangular sub-matrix whose sum is 0"/>
+    <hyperlink ref="B462" r:id="rId403" display="Boolean Parenthesization Problem"/>
+    <hyperlink ref="B471" r:id="rId404" display="Count set bits in an integer"/>
+    <hyperlink ref="B472" r:id="rId405" display="Find the two non-repeating elements in an array of repeating elements"/>
+    <hyperlink ref="B473" r:id="rId406" display="Count number of bits to be flipped to convert A to B"/>
+    <hyperlink ref="B474" r:id="rId407" display="Count total set bits in all numbers from 1 to n"/>
+    <hyperlink ref="B475" r:id="rId408" display="Program to find whether a no is power of two"/>
+    <hyperlink ref="B476" r:id="rId409" display="Find position of the only set bit"/>
+    <hyperlink ref="B477" r:id="rId410" display="Copy set bits in a range"/>
+    <hyperlink ref="B480" r:id="rId411" display="Power Set"/>
+    <hyperlink ref="B478" r:id="rId412" display="Divide two integers without using multiplication, division and mod operator"/>
+    <hyperlink ref="B479" r:id="rId413" display="Calculate square of a number without using *, / and pow()"/>
     <hyperlink ref="B356" r:id="rId414" display="Create a Graph, print it"/>
     <hyperlink ref="B38" r:id="rId415" display="Minimum swaps required bring elements less equal K together"/>
     <hyperlink ref="B2" r:id="rId416" display="Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw "/>

</xml_diff>

<commit_message>
[COMPLETE]Graphs: Solved 5 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="C392" sqref="C392"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="D398" sqref="D398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7160,7 +7160,7 @@
       <c r="B379" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="C379" s="18"/>
+      <c r="C379" s="17"/>
       <c r="D379" s="8"/>
     </row>
     <row r="380" ht="21" spans="1:4">
@@ -7299,27 +7299,27 @@
       <c r="A393" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B393" s="13" t="s">
+      <c r="B393" s="10" t="s">
         <v>518</v>
       </c>
-      <c r="C393" s="18"/>
+      <c r="C393" s="14"/>
       <c r="D393" s="8"/>
     </row>
     <row r="394" ht="21" spans="1:4">
       <c r="A394" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B394" s="13" t="s">
+      <c r="B394" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="C394" s="18"/>
+      <c r="C394" s="14"/>
       <c r="D394" s="8"/>
     </row>
     <row r="395" ht="21" spans="1:4">
       <c r="A395" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B395" s="13" t="s">
+      <c r="B395" s="10" t="s">
         <v>520</v>
       </c>
       <c r="C395" s="18"/>
@@ -7329,30 +7329,32 @@
       <c r="A396" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B396" s="13" t="s">
+      <c r="B396" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="C396" s="18"/>
+      <c r="C396" s="14"/>
       <c r="D396" s="8"/>
     </row>
     <row r="397" ht="21" spans="1:4">
       <c r="A397" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B397" s="13" t="s">
+      <c r="B397" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="C397" s="18"/>
+      <c r="C397" s="14"/>
       <c r="D397" s="8"/>
     </row>
     <row r="398" ht="21" spans="1:4">
       <c r="A398" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B398" s="13" t="s">
+      <c r="B398" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="C398" s="18"/>
+      <c r="C398" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D398" s="8"/>
     </row>
     <row r="399" ht="21" spans="2:4">

</xml_diff>

<commit_message>
[Trie]: Solved 4 questions, [DP]: Solved 16 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="D398" sqref="D398"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7374,14 +7374,14 @@
       <c r="B401" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="C401" s="18"/>
+      <c r="C401" s="14"/>
       <c r="D401" s="8"/>
     </row>
     <row r="402" ht="21" spans="1:4">
       <c r="A402" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="B402" s="13" t="s">
+      <c r="B402" s="10" t="s">
         <v>526</v>
       </c>
       <c r="C402" s="18"/>
@@ -7391,17 +7391,17 @@
       <c r="A403" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="B403" s="13" t="s">
+      <c r="B403" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="C403" s="18"/>
+      <c r="C403" s="14"/>
       <c r="D403" s="8"/>
     </row>
     <row r="404" ht="21" spans="1:4">
       <c r="A404" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="B404" s="13" t="s">
+      <c r="B404" s="10" t="s">
         <v>165</v>
       </c>
       <c r="C404" s="18"/>
@@ -7411,20 +7411,20 @@
       <c r="A405" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="B405" s="13" t="s">
+      <c r="B405" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="C405" s="18"/>
+      <c r="C405" s="14"/>
       <c r="D405" s="8"/>
     </row>
     <row r="406" ht="21" spans="1:4">
       <c r="A406" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="B406" s="13" t="s">
+      <c r="B406" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="C406" s="18"/>
+      <c r="C406" s="14"/>
       <c r="D406" s="8"/>
     </row>
     <row r="407" ht="21" spans="2:4">
@@ -7441,17 +7441,17 @@
       <c r="A409" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B409" s="13" t="s">
+      <c r="B409" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="C409" s="18"/>
+      <c r="C409" s="14"/>
       <c r="D409" s="8"/>
     </row>
     <row r="410" ht="21" spans="1:4">
       <c r="A410" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B410" s="13" t="s">
+      <c r="B410" s="10" t="s">
         <v>532</v>
       </c>
       <c r="C410" s="18"/>
@@ -7461,67 +7461,75 @@
       <c r="A411" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B411" s="13" t="s">
+      <c r="B411" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="C411" s="18"/>
+      <c r="C411" s="14"/>
       <c r="D411" s="8"/>
     </row>
     <row r="412" ht="21" spans="1:4">
       <c r="A412" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B412" s="13" t="s">
+      <c r="B412" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="C412" s="18"/>
+      <c r="C412" s="14"/>
       <c r="D412" s="8"/>
     </row>
     <row r="413" ht="21" spans="1:4">
       <c r="A413" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B413" s="13" t="s">
+      <c r="B413" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="C413" s="18"/>
+      <c r="C413" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D413" s="8"/>
     </row>
     <row r="414" ht="21" spans="1:4">
       <c r="A414" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B414" s="13" t="s">
+      <c r="B414" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="C414" s="18"/>
+      <c r="C414" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="D414" s="8"/>
     </row>
     <row r="415" ht="21" spans="1:4">
       <c r="A415" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B415" s="13" t="s">
+      <c r="B415" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="C415" s="18"/>
+      <c r="C415" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D415" s="8"/>
     </row>
     <row r="416" ht="21" spans="1:4">
       <c r="A416" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B416" s="13" t="s">
+      <c r="B416" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="C416" s="18"/>
+      <c r="C416" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D416" s="8"/>
     </row>
     <row r="417" ht="21" spans="1:4">
       <c r="A417" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B417" s="13" t="s">
+      <c r="B417" s="10" t="s">
         <v>538</v>
       </c>
       <c r="C417" s="18"/>
@@ -7531,17 +7539,17 @@
       <c r="A418" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B418" s="13" t="s">
+      <c r="B418" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="C418" s="18"/>
+      <c r="C418" s="14"/>
       <c r="D418" s="8"/>
     </row>
     <row r="419" ht="21" spans="1:4">
       <c r="A419" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B419" s="13" t="s">
+      <c r="B419" s="10" t="s">
         <v>540</v>
       </c>
       <c r="C419" s="18"/>
@@ -7551,40 +7559,42 @@
       <c r="A420" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B420" s="13" t="s">
+      <c r="B420" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="C420" s="18"/>
+      <c r="C420" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D420" s="8"/>
     </row>
     <row r="421" ht="21" spans="1:4">
       <c r="A421" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B421" s="13" t="s">
+      <c r="B421" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="C421" s="18"/>
+      <c r="C421" s="14"/>
       <c r="D421" s="8"/>
     </row>
     <row r="422" ht="21" spans="1:4">
       <c r="A422" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B422" s="13" t="s">
+      <c r="B422" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="C422" s="18"/>
+      <c r="C422" s="14"/>
       <c r="D422" s="8"/>
     </row>
     <row r="423" ht="21" spans="1:4">
       <c r="A423" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B423" s="13" t="s">
+      <c r="B423" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="C423" s="18"/>
+      <c r="C423" s="14"/>
       <c r="D423" s="8"/>
     </row>
     <row r="424" ht="21" spans="1:4">
@@ -7594,14 +7604,14 @@
       <c r="B424" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="C424" s="18"/>
+      <c r="C424" s="14"/>
       <c r="D424" s="8"/>
     </row>
     <row r="425" ht="21" spans="1:4">
       <c r="A425" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B425" s="13" t="s">
+      <c r="B425" s="10" t="s">
         <v>546</v>
       </c>
       <c r="C425" s="18"/>
@@ -7611,10 +7621,10 @@
       <c r="A426" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B426" s="13" t="s">
+      <c r="B426" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="C426" s="18"/>
+      <c r="C426" s="14"/>
       <c r="D426" s="8"/>
     </row>
     <row r="427" ht="21" spans="1:4">
@@ -7781,10 +7791,10 @@
       <c r="A443" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B443" s="13" t="s">
+      <c r="B443" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="C443" s="18"/>
+      <c r="C443" s="14"/>
       <c r="D443" s="8"/>
     </row>
     <row r="444" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[Dynamic Programming]: Solved 15 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1782,7 +1782,7 @@
     <t>Largest Independent Set Problem</t>
   </si>
   <si>
-    <t>Partition problem</t>
+    <t>Partition problem (Equal Subset Sum)</t>
   </si>
   <si>
     <t>Longest Palindromic Subsequence</t>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
+      <selection activeCell="C445" sqref="C445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7631,17 +7631,17 @@
       <c r="A427" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B427" s="13" t="s">
+      <c r="B427" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="C427" s="18"/>
+      <c r="C427" s="14"/>
       <c r="D427" s="8"/>
     </row>
     <row r="428" ht="21" spans="1:4">
       <c r="A428" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B428" s="13" t="s">
+      <c r="B428" s="10" t="s">
         <v>549</v>
       </c>
       <c r="C428" s="18"/>
@@ -7651,20 +7651,20 @@
       <c r="A429" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B429" s="13" t="s">
+      <c r="B429" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="C429" s="18"/>
+      <c r="C429" s="14"/>
       <c r="D429" s="8"/>
     </row>
     <row r="430" ht="21" spans="1:4">
       <c r="A430" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B430" s="13" t="s">
+      <c r="B430" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="C430" s="18"/>
+      <c r="C430" s="14"/>
       <c r="D430" s="8"/>
     </row>
     <row r="431" ht="21" spans="1:4">
@@ -7761,10 +7761,10 @@
       <c r="A440" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B440" s="13" t="s">
+      <c r="B440" s="10" t="s">
         <v>561</v>
       </c>
-      <c r="C440" s="18"/>
+      <c r="C440" s="14"/>
       <c r="D440" s="8"/>
     </row>
     <row r="441" ht="21" spans="1:4">
@@ -7801,20 +7801,20 @@
       <c r="A444" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B444" s="13" t="s">
+      <c r="B444" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="C444" s="18"/>
+      <c r="C444" s="14"/>
       <c r="D444" s="8"/>
     </row>
     <row r="445" ht="21" spans="1:4">
       <c r="A445" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B445" s="13" t="s">
+      <c r="B445" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="C445" s="18"/>
+      <c r="C445" s="14"/>
       <c r="D445" s="8"/>
     </row>
     <row r="446" ht="21" spans="1:4">
@@ -7841,20 +7841,20 @@
       <c r="A448" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B448" s="13" t="s">
+      <c r="B448" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="C448" s="18"/>
+      <c r="C448" s="14"/>
       <c r="D448" s="8"/>
     </row>
     <row r="449" ht="21" spans="1:4">
       <c r="A449" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B449" s="13" t="s">
+      <c r="B449" s="10" t="s">
         <v>570</v>
       </c>
-      <c r="C449" s="18"/>
+      <c r="C449" s="14"/>
       <c r="D449" s="8"/>
     </row>
     <row r="450" ht="21" spans="1:4">
@@ -8570,7 +8570,7 @@
     <hyperlink ref="B445" r:id="rId385" display="Unbounded Knapsack (Repetition of items allowed)"/>
     <hyperlink ref="B446" r:id="rId59" display="Word Break Problem"/>
     <hyperlink ref="B447" r:id="rId386" display="Largest Independent Set Problem"/>
-    <hyperlink ref="B448" r:id="rId250" display="Partition problem"/>
+    <hyperlink ref="B448" r:id="rId250" display="Partition problem (Equal Subset Sum)"/>
     <hyperlink ref="B450" r:id="rId64" display="Count All Palindromic Subsequence in a given String"/>
     <hyperlink ref="B449" r:id="rId387" display="Longest Palindromic Subsequence"/>
     <hyperlink ref="B451" r:id="rId388" display="Longest Palindromic Substring"/>

</xml_diff>

<commit_message>
[Dynamic Programming]: Solved 14 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="C445" sqref="C445"/>
+    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
+      <selection activeCell="C439" sqref="C439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7454,7 +7454,7 @@
       <c r="B410" s="10" t="s">
         <v>532</v>
       </c>
-      <c r="C410" s="18"/>
+      <c r="C410" s="14"/>
       <c r="D410" s="8"/>
     </row>
     <row r="411" ht="21" spans="1:4">
@@ -7644,7 +7644,7 @@
       <c r="B428" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="C428" s="18"/>
+      <c r="C428" s="14"/>
       <c r="D428" s="8"/>
     </row>
     <row r="429" ht="21" spans="1:4">
@@ -7681,10 +7681,10 @@
       <c r="A432" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B432" s="13" t="s">
+      <c r="B432" s="10" t="s">
         <v>553</v>
       </c>
-      <c r="C432" s="18"/>
+      <c r="C432" s="14"/>
       <c r="D432" s="8"/>
     </row>
     <row r="433" ht="21" spans="1:4">
@@ -7701,60 +7701,60 @@
       <c r="A434" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B434" s="13" t="s">
+      <c r="B434" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="C434" s="18"/>
+      <c r="C434" s="14"/>
       <c r="D434" s="8"/>
     </row>
     <row r="435" ht="21" spans="1:4">
       <c r="A435" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B435" s="13" t="s">
+      <c r="B435" s="10" t="s">
         <v>556</v>
       </c>
-      <c r="C435" s="18"/>
+      <c r="C435" s="14"/>
       <c r="D435" s="8"/>
     </row>
     <row r="436" ht="21" spans="1:4">
       <c r="A436" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B436" s="13" t="s">
+      <c r="B436" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="C436" s="18"/>
+      <c r="C436" s="14"/>
       <c r="D436" s="8"/>
     </row>
     <row r="437" ht="21" spans="1:4">
       <c r="A437" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B437" s="13" t="s">
+      <c r="B437" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="C437" s="18"/>
+      <c r="C437" s="14"/>
       <c r="D437" s="8"/>
     </row>
     <row r="438" ht="21" spans="1:4">
       <c r="A438" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B438" s="13" t="s">
+      <c r="B438" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="C438" s="18"/>
+      <c r="C438" s="14"/>
       <c r="D438" s="8"/>
     </row>
     <row r="439" ht="21" spans="1:4">
       <c r="A439" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B439" s="13" t="s">
+      <c r="B439" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="C439" s="18"/>
+      <c r="C439" s="14"/>
       <c r="D439" s="8"/>
     </row>
     <row r="440" ht="21" spans="1:4">
@@ -7771,10 +7771,10 @@
       <c r="A441" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B441" s="13" t="s">
+      <c r="B441" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="C441" s="18"/>
+      <c r="C441" s="14"/>
       <c r="D441" s="8"/>
     </row>
     <row r="442" ht="21" spans="1:4">
@@ -7871,10 +7871,10 @@
       <c r="A451" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B451" s="13" t="s">
+      <c r="B451" s="10" t="s">
         <v>572</v>
       </c>
-      <c r="C451" s="18"/>
+      <c r="C451" s="14"/>
       <c r="D451" s="8"/>
     </row>
     <row r="452" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[Dynamic Programming]: Solved 13 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1883,10 +1883,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1969,7 +1969,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1984,37 +2007,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2038,7 +2030,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2047,13 +2061,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2068,14 +2075,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2089,7 +2089,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2098,14 +2106,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2156,13 +2156,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2174,55 +2234,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2240,19 +2252,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2270,55 +2300,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2330,7 +2324,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2397,6 +2397,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2422,41 +2452,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2478,145 +2478,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
-      <selection activeCell="C439" sqref="C439"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="C433" sqref="C433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7187,7 +7187,7 @@
       <c r="A382" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B382" s="13" t="s">
+      <c r="B382" s="10" t="s">
         <v>507</v>
       </c>
       <c r="C382" s="18"/>
@@ -7496,7 +7496,7 @@
       <c r="B414" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="C414" s="18" t="s">
+      <c r="C414" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D414" s="8"/>
@@ -7691,10 +7691,10 @@
       <c r="A433" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B433" s="13" t="s">
+      <c r="B433" s="10" t="s">
         <v>554</v>
       </c>
-      <c r="C433" s="18"/>
+      <c r="C433" s="14"/>
       <c r="D433" s="8"/>
     </row>
     <row r="434" ht="21" spans="1:4">
@@ -7821,17 +7821,17 @@
       <c r="A446" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B446" s="13" t="s">
+      <c r="B446" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="C446" s="18"/>
+      <c r="C446" s="14"/>
       <c r="D446" s="8"/>
     </row>
     <row r="447" ht="21" spans="1:4">
       <c r="A447" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B447" s="13" t="s">
+      <c r="B447" s="10" t="s">
         <v>568</v>
       </c>
       <c r="C447" s="18"/>
@@ -7881,30 +7881,30 @@
       <c r="A452" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B452" s="13" t="s">
+      <c r="B452" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="C452" s="18"/>
+      <c r="C452" s="14"/>
       <c r="D452" s="8"/>
     </row>
     <row r="453" ht="21" spans="1:4">
       <c r="A453" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B453" s="13" t="s">
+      <c r="B453" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="C453" s="18"/>
+      <c r="C453" s="14"/>
       <c r="D453" s="8"/>
     </row>
     <row r="454" ht="21" spans="1:4">
       <c r="A454" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B454" s="13" t="s">
+      <c r="B454" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="C454" s="18"/>
+      <c r="C454" s="14"/>
       <c r="D454" s="8"/>
     </row>
     <row r="455" ht="21" spans="1:4">
@@ -7921,10 +7921,10 @@
       <c r="A456" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B456" s="13" t="s">
+      <c r="B456" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="C456" s="18"/>
+      <c r="C456" s="14"/>
       <c r="D456" s="8"/>
     </row>
     <row r="457" ht="21" spans="1:4">
@@ -7951,7 +7951,7 @@
       <c r="A459" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B459" s="13" t="s">
+      <c r="B459" s="10" t="s">
         <v>580</v>
       </c>
       <c r="C459" s="18"/>
@@ -8021,20 +8021,22 @@
       <c r="A466" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B466" s="13" t="s">
+      <c r="B466" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="C466" s="18"/>
+      <c r="C466" s="14"/>
       <c r="D466" s="8"/>
     </row>
     <row r="467" ht="21" spans="1:4">
       <c r="A467" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B467" s="13" t="s">
+      <c r="B467" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="C467" s="18"/>
+      <c r="C467" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D467" s="8"/>
     </row>
     <row r="468" ht="21" spans="1:4">
@@ -8044,7 +8046,7 @@
       <c r="B468" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="C468" s="18"/>
+      <c r="C468" s="14"/>
       <c r="D468" s="8"/>
     </row>
     <row r="469" ht="21" spans="2:4">

</xml_diff>

<commit_message>
[Dynamic Programming]: Solved 8 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1884,8 +1884,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="31">
@@ -1968,10 +1968,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1983,39 +1991,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2030,21 +2022,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2053,6 +2030,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2082,22 +2074,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2105,7 +2105,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2156,7 +2156,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2168,115 +2288,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2294,49 +2312,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2374,6 +2374,21 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2460,163 +2475,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C433" sqref="C433"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="C461" sqref="C461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7931,17 +7931,17 @@
       <c r="A457" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B457" s="13" t="s">
+      <c r="B457" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="C457" s="18"/>
+      <c r="C457" s="14"/>
       <c r="D457" s="8"/>
     </row>
     <row r="458" ht="21" spans="1:4">
       <c r="A458" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B458" s="13" t="s">
+      <c r="B458" s="10" t="s">
         <v>579</v>
       </c>
       <c r="C458" s="18"/>
@@ -7954,67 +7954,67 @@
       <c r="B459" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="C459" s="18"/>
+      <c r="C459" s="14"/>
       <c r="D459" s="8"/>
     </row>
     <row r="460" ht="21" spans="1:4">
       <c r="A460" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B460" s="13" t="s">
+      <c r="B460" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="C460" s="18"/>
+      <c r="C460" s="14"/>
       <c r="D460" s="8"/>
     </row>
     <row r="461" ht="21" spans="1:4">
       <c r="A461" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B461" s="13" t="s">
+      <c r="B461" s="10" t="s">
         <v>582</v>
       </c>
-      <c r="C461" s="18"/>
+      <c r="C461" s="14"/>
       <c r="D461" s="8"/>
     </row>
     <row r="462" ht="21" spans="1:4">
       <c r="A462" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B462" s="13" t="s">
+      <c r="B462" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="C462" s="18"/>
+      <c r="C462" s="14"/>
       <c r="D462" s="8"/>
     </row>
     <row r="463" ht="21" spans="1:4">
       <c r="A463" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B463" s="13" t="s">
+      <c r="B463" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="C463" s="18"/>
+      <c r="C463" s="14"/>
       <c r="D463" s="8"/>
     </row>
     <row r="464" ht="21" spans="1:4">
       <c r="A464" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B464" s="13" t="s">
+      <c r="B464" s="10" t="s">
         <v>585</v>
       </c>
-      <c r="C464" s="18"/>
+      <c r="C464" s="14"/>
       <c r="D464" s="8"/>
     </row>
     <row r="465" ht="21" spans="1:4">
       <c r="A465" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="B465" s="13" t="s">
+      <c r="B465" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="C465" s="18"/>
+      <c r="C465" s="14"/>
       <c r="D465" s="8"/>
     </row>
     <row r="466" ht="21" spans="1:4">

</xml_diff>

<commit_message>
[COMPLETE]Bit Manipulation: Solved 10 questions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="601">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2987,8 +2987,8 @@
   <sheetPr/>
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A442" workbookViewId="0">
-      <selection activeCell="C461" sqref="C461"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A462" workbookViewId="0">
+      <selection activeCell="C473" sqref="C473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -6578,7 +6578,9 @@
       <c r="B321" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="C321" s="18"/>
+      <c r="C321" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D321" s="8"/>
     </row>
     <row r="322" ht="21" spans="1:4">
@@ -6797,10 +6799,10 @@
       <c r="A343" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B343" s="13" t="s">
+      <c r="B343" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="C343" s="18"/>
+      <c r="C343" s="14"/>
       <c r="D343" s="8"/>
     </row>
     <row r="344" ht="21" spans="1:4">
@@ -6875,7 +6877,7 @@
       <c r="A350" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="B350" s="13" t="s">
+      <c r="B350" s="10" t="s">
         <v>475</v>
       </c>
       <c r="C350" s="18"/>
@@ -8064,30 +8066,30 @@
       <c r="A471" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="B471" s="13" t="s">
+      <c r="B471" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="C471" s="18"/>
+      <c r="C471" s="14"/>
       <c r="D471" s="8"/>
     </row>
     <row r="472" ht="21" spans="1:4">
       <c r="A472" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="B472" s="13" t="s">
+      <c r="B472" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="C472" s="18"/>
+      <c r="C472" s="14"/>
       <c r="D472" s="8"/>
     </row>
     <row r="473" ht="21" spans="1:4">
       <c r="A473" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="B473" s="13" t="s">
+      <c r="B473" s="10" t="s">
         <v>593</v>
       </c>
-      <c r="C473" s="18"/>
+      <c r="C473" s="14"/>
       <c r="D473" s="8"/>
     </row>
     <row r="474" ht="21" spans="1:4">

</xml_diff>